<commit_message>
fix import issue on SA
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20201216.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20201216.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="578">
   <si>
     <t>Acronym</t>
   </si>
@@ -2267,6 +2267,9 @@
   <si>
     <t>Number of Agglomeration</t>
   </si>
+  <si>
+    <t>NI</t>
+  </si>
 </sst>
 </file>
 
@@ -2795,7 +2798,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5395,14 +5398,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="40" fillId="37" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="23" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5906,6 +5903,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="56" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6541,8 +6544,8 @@
       </c>
       <c r="C2" s="392"/>
       <c r="D2" s="392"/>
-      <c r="E2" s="863"/>
-      <c r="F2" s="863"/>
+      <c r="E2" s="859"/>
+      <c r="F2" s="859"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="391"/>
@@ -6574,13 +6577,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="389"/>
-      <c r="B6" s="864" t="s">
+      <c r="B6" s="860" t="s">
         <v>514</v>
       </c>
-      <c r="C6" s="864"/>
-      <c r="D6" s="864"/>
-      <c r="E6" s="864"/>
-      <c r="F6" s="864"/>
+      <c r="C6" s="860"/>
+      <c r="D6" s="860"/>
+      <c r="E6" s="860"/>
+      <c r="F6" s="860"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="389"/>
@@ -6595,14 +6598,14 @@
       <c r="B8" s="418" t="s">
         <v>551</v>
       </c>
-      <c r="C8" s="875" t="s">
+      <c r="C8" s="871" t="s">
         <v>293</v>
       </c>
-      <c r="D8" s="876"/>
-      <c r="E8" s="875" t="s">
+      <c r="D8" s="872"/>
+      <c r="E8" s="871" t="s">
         <v>294</v>
       </c>
-      <c r="F8" s="876"/>
+      <c r="F8" s="872"/>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="389"/>
@@ -6738,11 +6741,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="389"/>
-      <c r="B22" s="869"/>
-      <c r="C22" s="869"/>
-      <c r="D22" s="869"/>
-      <c r="E22" s="869"/>
-      <c r="F22" s="869"/>
+      <c r="B22" s="865"/>
+      <c r="C22" s="865"/>
+      <c r="D22" s="865"/>
+      <c r="E22" s="865"/>
+      <c r="F22" s="865"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="389"/>
@@ -6813,13 +6816,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="877" t="s">
+      <c r="B2" s="873" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="878" t="s">
+      <c r="C2" s="874" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="878" t="s">
+      <c r="D2" s="874" t="s">
         <v>225</v>
       </c>
       <c r="E2" s="443" t="s">
@@ -6854,9 +6857,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="877"/>
-      <c r="C3" s="879"/>
-      <c r="D3" s="879"/>
+      <c r="B3" s="873"/>
+      <c r="C3" s="875"/>
+      <c r="D3" s="875"/>
       <c r="E3" s="458" t="s">
         <v>355</v>
       </c>
@@ -6889,7 +6892,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="880" t="s">
+      <c r="B4" s="876" t="s">
         <v>358</v>
       </c>
       <c r="C4" s="444" t="s">
@@ -6908,7 +6911,7 @@
       <c r="N4" s="446"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="880"/>
+      <c r="B5" s="876"/>
       <c r="C5" s="444" t="s">
         <v>135</v>
       </c>
@@ -6925,7 +6928,7 @@
       <c r="N5" s="446"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="881"/>
+      <c r="B6" s="877"/>
       <c r="C6" s="454" t="s">
         <v>348</v>
       </c>
@@ -7039,43 +7042,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="885" t="s">
+      <c r="A1" s="881" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="886"/>
+      <c r="B1" s="882"/>
       <c r="C1" s="474"/>
-      <c r="D1" s="896" t="s">
+      <c r="D1" s="892" t="s">
         <v>360</v>
       </c>
-      <c r="E1" s="897"/>
-      <c r="F1" s="897"/>
-      <c r="G1" s="897"/>
-      <c r="H1" s="897"/>
-      <c r="I1" s="898"/>
-      <c r="J1" s="887" t="s">
+      <c r="E1" s="893"/>
+      <c r="F1" s="893"/>
+      <c r="G1" s="893"/>
+      <c r="H1" s="893"/>
+      <c r="I1" s="894"/>
+      <c r="J1" s="883" t="s">
         <v>361</v>
       </c>
-      <c r="K1" s="888"/>
-      <c r="L1" s="888"/>
-      <c r="M1" s="888"/>
-      <c r="N1" s="889"/>
-      <c r="O1" s="890" t="s">
+      <c r="K1" s="884"/>
+      <c r="L1" s="884"/>
+      <c r="M1" s="884"/>
+      <c r="N1" s="885"/>
+      <c r="O1" s="886" t="s">
         <v>362</v>
       </c>
-      <c r="P1" s="891"/>
-      <c r="Q1" s="892"/>
+      <c r="P1" s="887"/>
+      <c r="Q1" s="888"/>
       <c r="R1" s="461" t="s">
         <v>122</v>
       </c>
       <c r="S1" s="462"/>
-      <c r="T1" s="884" t="s">
+      <c r="T1" s="880" t="s">
         <v>562</v>
       </c>
-      <c r="U1" s="884"/>
-      <c r="V1" s="884"/>
-      <c r="W1" s="884"/>
-      <c r="X1" s="884"/>
-      <c r="Y1" s="884"/>
+      <c r="U1" s="880"/>
+      <c r="V1" s="880"/>
+      <c r="W1" s="880"/>
+      <c r="X1" s="880"/>
+      <c r="Y1" s="880"/>
     </row>
     <row r="2" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="464" t="s">
@@ -7087,18 +7090,18 @@
       <c r="C2" s="465" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="901" t="s">
+      <c r="D2" s="897" t="s">
         <v>364</v>
       </c>
-      <c r="E2" s="900"/>
-      <c r="F2" s="900" t="s">
+      <c r="E2" s="896"/>
+      <c r="F2" s="896" t="s">
         <v>365</v>
       </c>
-      <c r="G2" s="900"/>
-      <c r="H2" s="899" t="s">
+      <c r="G2" s="896"/>
+      <c r="H2" s="895" t="s">
         <v>366</v>
       </c>
-      <c r="I2" s="899"/>
+      <c r="I2" s="895"/>
       <c r="J2" s="466">
         <v>0</v>
       </c>
@@ -7129,18 +7132,18 @@
       <c r="S2" s="706" t="s">
         <v>133</v>
       </c>
-      <c r="T2" s="882" t="s">
+      <c r="T2" s="878" t="s">
         <v>526</v>
       </c>
-      <c r="U2" s="882"/>
-      <c r="V2" s="883" t="s">
+      <c r="U2" s="878"/>
+      <c r="V2" s="879" t="s">
         <v>548</v>
       </c>
-      <c r="W2" s="883"/>
-      <c r="X2" s="883" t="s">
+      <c r="W2" s="879"/>
+      <c r="X2" s="879" t="s">
         <v>549</v>
       </c>
-      <c r="Y2" s="883"/>
+      <c r="Y2" s="879"/>
     </row>
     <row r="3" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="469"/>
@@ -7166,13 +7169,13 @@
       <c r="I3" s="690" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="893" t="s">
+      <c r="J3" s="889" t="s">
         <v>371</v>
       </c>
-      <c r="K3" s="894"/>
-      <c r="L3" s="894"/>
-      <c r="M3" s="894"/>
-      <c r="N3" s="895"/>
+      <c r="K3" s="890"/>
+      <c r="L3" s="890"/>
+      <c r="M3" s="890"/>
+      <c r="N3" s="891"/>
       <c r="O3" s="477"/>
       <c r="P3" s="477"/>
       <c r="Q3" s="477"/>
@@ -8452,25 +8455,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="782" t="s">
+      <c r="A1" s="778" t="s">
         <v>372</v>
       </c>
-      <c r="B1" s="783"/>
-      <c r="C1" s="783"/>
-      <c r="D1" s="783"/>
-      <c r="E1" s="783"/>
-      <c r="F1" s="783"/>
+      <c r="B1" s="779"/>
+      <c r="C1" s="779"/>
+      <c r="D1" s="779"/>
+      <c r="E1" s="779"/>
+      <c r="F1" s="779"/>
       <c r="G1" s="491"/>
-      <c r="H1" s="908" t="s">
+      <c r="H1" s="904" t="s">
         <v>216</v>
       </c>
-      <c r="I1" s="909"/>
-      <c r="J1" s="909"/>
+      <c r="I1" s="905"/>
+      <c r="J1" s="905"/>
       <c r="K1" s="493"/>
       <c r="L1" s="483"/>
       <c r="M1" s="493"/>
       <c r="N1" s="484"/>
-      <c r="O1" s="906" t="s">
+      <c r="O1" s="902" t="s">
         <v>373</v>
       </c>
       <c r="P1" s="485"/>
@@ -8482,26 +8485,26 @@
       <c r="T1" s="483"/>
       <c r="U1" s="493"/>
       <c r="V1" s="484"/>
-      <c r="W1" s="906" t="s">
+      <c r="W1" s="902" t="s">
         <v>375</v>
       </c>
       <c r="X1" s="485"/>
-      <c r="Y1" s="910" t="s">
+      <c r="Y1" s="906" t="s">
         <v>376</v>
       </c>
-      <c r="Z1" s="910"/>
-      <c r="AA1" s="910"/>
-      <c r="AB1" s="910"/>
-      <c r="AC1" s="910"/>
-      <c r="AD1" s="911"/>
-      <c r="AE1" s="906" t="s">
+      <c r="Z1" s="906"/>
+      <c r="AA1" s="906"/>
+      <c r="AB1" s="906"/>
+      <c r="AC1" s="906"/>
+      <c r="AD1" s="907"/>
+      <c r="AE1" s="902" t="s">
         <v>377</v>
       </c>
-      <c r="AF1" s="905" t="s">
+      <c r="AF1" s="901" t="s">
         <v>547</v>
       </c>
-      <c r="AG1" s="884"/>
-      <c r="AH1" s="884"/>
+      <c r="AG1" s="880"/>
+      <c r="AH1" s="880"/>
       <c r="AI1" s="713"/>
       <c r="AJ1" s="713"/>
       <c r="AK1" s="713"/>
@@ -8560,56 +8563,56 @@
       <c r="C2" s="492" t="s">
         <v>379</v>
       </c>
-      <c r="D2" s="904" t="s">
+      <c r="D2" s="900" t="s">
         <v>552</v>
       </c>
-      <c r="E2" s="904"/>
-      <c r="F2" s="904" t="s">
+      <c r="E2" s="900"/>
+      <c r="F2" s="900" t="s">
         <v>553</v>
       </c>
-      <c r="G2" s="904"/>
+      <c r="G2" s="900"/>
       <c r="H2" s="487"/>
-      <c r="I2" s="902" t="s">
+      <c r="I2" s="898" t="s">
         <v>235</v>
       </c>
-      <c r="J2" s="902"/>
-      <c r="K2" s="902" t="s">
+      <c r="J2" s="898"/>
+      <c r="K2" s="898" t="s">
         <v>236</v>
       </c>
-      <c r="L2" s="902"/>
-      <c r="M2" s="902" t="s">
+      <c r="L2" s="898"/>
+      <c r="M2" s="898" t="s">
         <v>237</v>
       </c>
-      <c r="N2" s="903"/>
-      <c r="O2" s="907"/>
+      <c r="N2" s="899"/>
+      <c r="O2" s="903"/>
       <c r="P2" s="488"/>
-      <c r="Q2" s="902" t="s">
+      <c r="Q2" s="898" t="s">
         <v>235</v>
       </c>
-      <c r="R2" s="902"/>
-      <c r="S2" s="902" t="s">
+      <c r="R2" s="898"/>
+      <c r="S2" s="898" t="s">
         <v>236</v>
       </c>
-      <c r="T2" s="902"/>
-      <c r="U2" s="902" t="s">
+      <c r="T2" s="898"/>
+      <c r="U2" s="898" t="s">
         <v>237</v>
       </c>
-      <c r="V2" s="903"/>
-      <c r="W2" s="907"/>
+      <c r="V2" s="899"/>
+      <c r="W2" s="903"/>
       <c r="X2" s="488"/>
-      <c r="Y2" s="902" t="s">
+      <c r="Y2" s="898" t="s">
         <v>235</v>
       </c>
-      <c r="Z2" s="902"/>
-      <c r="AA2" s="902" t="s">
+      <c r="Z2" s="898"/>
+      <c r="AA2" s="898" t="s">
         <v>236</v>
       </c>
-      <c r="AB2" s="902"/>
-      <c r="AC2" s="902" t="s">
+      <c r="AB2" s="898"/>
+      <c r="AC2" s="898" t="s">
         <v>237</v>
       </c>
-      <c r="AD2" s="903"/>
-      <c r="AE2" s="907"/>
+      <c r="AD2" s="899"/>
+      <c r="AE2" s="903"/>
       <c r="AF2" s="707" t="s">
         <v>526</v>
       </c>
@@ -9703,7 +9706,7 @@
   <dimension ref="A1:U179"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9727,55 +9730,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="912"/>
-      <c r="B1" s="813"/>
-      <c r="C1" s="813"/>
+      <c r="A1" s="908"/>
+      <c r="B1" s="809"/>
+      <c r="C1" s="809"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="J2" s="766" t="s">
+      <c r="I2" s="936"/>
+      <c r="J2" s="937" t="s">
         <v>554</v>
       </c>
-      <c r="K2" s="766" t="s">
+      <c r="K2" s="937" t="s">
         <v>406</v>
       </c>
-      <c r="L2" s="766" t="s">
+      <c r="L2" s="937" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="920" t="s">
+      <c r="A3" s="916" t="s">
         <v>405</v>
       </c>
-      <c r="B3" s="922" t="s">
+      <c r="B3" s="918" t="s">
         <v>515</v>
       </c>
-      <c r="C3" s="923"/>
-      <c r="D3" s="918" t="s">
+      <c r="C3" s="919"/>
+      <c r="D3" s="914" t="s">
         <v>516</v>
       </c>
-      <c r="E3" s="919"/>
-      <c r="F3" s="918" t="s">
+      <c r="E3" s="915"/>
+      <c r="F3" s="914" t="s">
         <v>555</v>
       </c>
-      <c r="G3" s="919"/>
-      <c r="I3" s="767" t="str">
+      <c r="G3" s="915"/>
+      <c r="I3" s="934" t="str">
         <f>$B$3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="J3" s="764" t="s">
+      <c r="J3" s="935" t="s">
         <v>571</v>
       </c>
-      <c r="K3" s="764"/>
-      <c r="L3" s="764"/>
+      <c r="K3" s="746"/>
+      <c r="L3" s="746"/>
       <c r="N3" s="731"/>
-      <c r="O3" s="934" t="s">
+      <c r="O3" s="930" t="s">
         <v>406</v>
       </c>
-      <c r="P3" s="934"/>
-      <c r="Q3" s="934" t="s">
+      <c r="P3" s="930"/>
+      <c r="Q3" s="930" t="s">
         <v>407</v>
       </c>
-      <c r="R3" s="934"/>
+      <c r="R3" s="930"/>
       <c r="S3" s="731"/>
       <c r="T3" s="739" t="s">
         <v>408</v>
@@ -9783,7 +9787,7 @@
       <c r="U3" s="731"/>
     </row>
     <row r="4" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="921"/>
+      <c r="A4" s="917"/>
       <c r="B4" s="531" t="s">
         <v>409</v>
       </c>
@@ -9802,15 +9806,15 @@
       <c r="G4" s="531" t="s">
         <v>410</v>
       </c>
-      <c r="I4" s="767" t="str">
-        <f t="shared" ref="I4:I6" si="0">$B$3</f>
+      <c r="I4" s="934" t="str">
+        <f t="shared" ref="I4:I7" si="0">$B$3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="J4" s="764" t="s">
+      <c r="J4" s="935" t="s">
         <v>572</v>
       </c>
-      <c r="K4" s="764"/>
-      <c r="L4" s="764"/>
+      <c r="K4" s="746"/>
+      <c r="L4" s="746"/>
       <c r="N4" s="739" t="s">
         <v>411</v>
       </c>
@@ -9850,15 +9854,15 @@
       <c r="E5" s="596"/>
       <c r="F5" s="603"/>
       <c r="G5" s="596"/>
-      <c r="I5" s="767" t="str">
+      <c r="I5" s="934" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="J5" s="764" t="s">
+      <c r="J5" s="935" t="s">
         <v>573</v>
       </c>
-      <c r="K5" s="764"/>
-      <c r="L5" s="764"/>
+      <c r="K5" s="746"/>
+      <c r="L5" s="746"/>
       <c r="N5" s="739" t="str">
         <f>A5</f>
         <v>2 000 - 10 000</v>
@@ -9899,15 +9903,15 @@
       <c r="E6" s="599"/>
       <c r="F6" s="603"/>
       <c r="G6" s="599"/>
-      <c r="I6" s="767" t="str">
+      <c r="I6" s="934" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="J6" s="764" t="s">
-        <v>574</v>
-      </c>
-      <c r="K6" s="764"/>
-      <c r="L6" s="764"/>
+      <c r="J6" s="935" t="s">
+        <v>577</v>
+      </c>
+      <c r="K6" s="746"/>
+      <c r="L6" s="746"/>
       <c r="N6" s="739" t="str">
         <f>A6</f>
         <v>10 001 - 100 000</v>
@@ -9948,15 +9952,15 @@
       <c r="E7" s="599"/>
       <c r="F7" s="603"/>
       <c r="G7" s="599"/>
-      <c r="I7" s="767" t="str">
-        <f>$D$3</f>
-        <v>[#previous_year#]</v>
-      </c>
-      <c r="J7" s="764" t="s">
-        <v>571</v>
-      </c>
-      <c r="K7" s="763"/>
-      <c r="L7" s="763"/>
+      <c r="I7" s="934" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[#current_year#] </v>
+      </c>
+      <c r="J7" s="935" t="s">
+        <v>574</v>
+      </c>
+      <c r="K7" s="746"/>
+      <c r="L7" s="746"/>
       <c r="N7" s="739" t="str">
         <f>A7</f>
         <v>&gt;100 000</v>
@@ -9988,15 +9992,15 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="I8" s="767" t="str">
-        <f t="shared" ref="I8:I10" si="2">$D$3</f>
+      <c r="I8" s="934" t="str">
+        <f>$D$3</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="J8" s="764" t="s">
-        <v>572</v>
-      </c>
-      <c r="K8" s="763"/>
-      <c r="L8" s="763"/>
+      <c r="J8" s="935" t="s">
+        <v>571</v>
+      </c>
+      <c r="K8" s="746"/>
+      <c r="L8" s="746"/>
       <c r="N8" s="739" t="s">
         <v>415</v>
       </c>
@@ -10021,46 +10025,46 @@
       <c r="U8" s="731"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="I9" s="767" t="str">
+      <c r="I9" s="934" t="str">
+        <f t="shared" ref="I9:I12" si="2">$D$3</f>
+        <v>[#previous_year#]</v>
+      </c>
+      <c r="J9" s="935" t="s">
+        <v>572</v>
+      </c>
+      <c r="K9" s="746"/>
+      <c r="L9" s="746"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="I10" s="934" t="str">
         <f t="shared" si="2"/>
         <v>[#previous_year#]</v>
       </c>
-      <c r="J9" s="764" t="s">
+      <c r="J10" s="935" t="s">
         <v>573</v>
       </c>
-      <c r="K9" s="763"/>
-      <c r="L9" s="763"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="I10" s="767" t="str">
+      <c r="K10" s="746"/>
+      <c r="L10" s="746"/>
+      <c r="N10" s="739"/>
+      <c r="O10" s="930" t="s">
+        <v>409</v>
+      </c>
+      <c r="P10" s="930"/>
+      <c r="Q10" s="930" t="s">
+        <v>416</v>
+      </c>
+      <c r="R10" s="930"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="I11" s="934" t="str">
         <f t="shared" si="2"/>
         <v>[#previous_year#]</v>
       </c>
-      <c r="J10" s="764" t="s">
-        <v>574</v>
-      </c>
-      <c r="K10" s="763"/>
-      <c r="L10" s="763"/>
-      <c r="N10" s="739"/>
-      <c r="O10" s="934" t="s">
-        <v>409</v>
-      </c>
-      <c r="P10" s="934"/>
-      <c r="Q10" s="934" t="s">
-        <v>416</v>
-      </c>
-      <c r="R10" s="934"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="I11" s="767" t="str">
-        <f>$F$3</f>
-        <v>[#previous_year_n2#]</v>
-      </c>
-      <c r="J11" s="764" t="s">
-        <v>571</v>
-      </c>
-      <c r="K11" s="763"/>
-      <c r="L11" s="763"/>
+      <c r="J11" s="935" t="s">
+        <v>577</v>
+      </c>
+      <c r="K11" s="746"/>
+      <c r="L11" s="746"/>
       <c r="N11" s="739" t="s">
         <v>405</v>
       </c>
@@ -10082,15 +10086,15 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="I12" s="767" t="str">
-        <f t="shared" ref="I12:I14" si="3">$F$3</f>
-        <v>[#previous_year_n2#]</v>
-      </c>
-      <c r="J12" s="764" t="s">
-        <v>572</v>
-      </c>
-      <c r="K12" s="763"/>
-      <c r="L12" s="763"/>
+      <c r="I12" s="934" t="str">
+        <f t="shared" si="2"/>
+        <v>[#previous_year#]</v>
+      </c>
+      <c r="J12" s="935" t="s">
+        <v>574</v>
+      </c>
+      <c r="K12" s="746"/>
+      <c r="L12" s="746"/>
       <c r="N12" s="739" t="str">
         <f>A5</f>
         <v>2 000 - 10 000</v>
@@ -10113,7 +10117,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="920" t="s">
+      <c r="A13" s="916" t="s">
         <v>417</v>
       </c>
       <c r="B13" s="530" t="str">
@@ -10128,15 +10132,15 @@
         <f>F3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="I13" s="767" t="str">
-        <f t="shared" si="3"/>
+      <c r="I13" s="934" t="str">
+        <f>$F$3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="J13" s="764" t="s">
-        <v>573</v>
-      </c>
-      <c r="K13" s="763"/>
-      <c r="L13" s="763"/>
+      <c r="J13" s="935" t="s">
+        <v>571</v>
+      </c>
+      <c r="K13" s="746"/>
+      <c r="L13" s="746"/>
       <c r="N13" s="739" t="str">
         <f>A6</f>
         <v>10 001 - 100 000</v>
@@ -10159,7 +10163,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="921"/>
+      <c r="A14" s="917"/>
       <c r="B14" s="533" t="s">
         <v>410</v>
       </c>
@@ -10169,15 +10173,15 @@
       <c r="D14" s="725" t="s">
         <v>410</v>
       </c>
-      <c r="I14" s="767" t="str">
-        <f t="shared" si="3"/>
+      <c r="I14" s="934" t="str">
+        <f t="shared" ref="I14:I17" si="3">$F$3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="J14" s="764" t="s">
-        <v>574</v>
-      </c>
-      <c r="K14" s="763"/>
-      <c r="L14" s="763"/>
+      <c r="J14" s="935" t="s">
+        <v>572</v>
+      </c>
+      <c r="K14" s="746"/>
+      <c r="L14" s="746"/>
       <c r="N14" s="739" t="str">
         <f>A7</f>
         <v>&gt;100 000</v>
@@ -10206,6 +10210,15 @@
       <c r="B15" s="539"/>
       <c r="C15" s="539"/>
       <c r="D15" s="603"/>
+      <c r="I15" s="934" t="str">
+        <f t="shared" si="3"/>
+        <v>[#previous_year_n2#]</v>
+      </c>
+      <c r="J15" s="935" t="s">
+        <v>573</v>
+      </c>
+      <c r="K15" s="746"/>
+      <c r="L15" s="746"/>
       <c r="N15" s="739" t="s">
         <v>415</v>
       </c>
@@ -10233,6 +10246,15 @@
       <c r="B16" s="539"/>
       <c r="C16" s="539"/>
       <c r="D16" s="603"/>
+      <c r="I16" s="934" t="str">
+        <f t="shared" si="3"/>
+        <v>[#previous_year_n2#]</v>
+      </c>
+      <c r="J16" s="935" t="s">
+        <v>577</v>
+      </c>
+      <c r="K16" s="746"/>
+      <c r="L16" s="746"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="532" t="s">
@@ -10241,6 +10263,15 @@
       <c r="B17" s="539"/>
       <c r="C17" s="539"/>
       <c r="D17" s="603"/>
+      <c r="I17" s="934" t="str">
+        <f t="shared" si="3"/>
+        <v>[#previous_year_n2#]</v>
+      </c>
+      <c r="J17" s="935" t="s">
+        <v>574</v>
+      </c>
+      <c r="K17" s="746"/>
+      <c r="L17" s="746"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="534" t="s">
@@ -10262,34 +10293,34 @@
       <c r="A21" s="521" t="s">
         <v>422</v>
       </c>
-      <c r="B21" s="936" t="s">
+      <c r="B21" s="932" t="s">
         <v>575</v>
       </c>
-      <c r="C21" s="937"/>
-      <c r="D21" s="937"/>
-      <c r="E21" s="937"/>
-      <c r="F21" s="937"/>
-      <c r="G21" s="937"/>
+      <c r="C21" s="933"/>
+      <c r="D21" s="933"/>
+      <c r="E21" s="933"/>
+      <c r="F21" s="933"/>
+      <c r="G21" s="933"/>
     </row>
     <row r="22" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="535" t="s">
         <v>386</v>
       </c>
-      <c r="B22" s="924" t="str">
+      <c r="B22" s="920" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C22" s="925"/>
-      <c r="D22" s="924" t="str">
+      <c r="C22" s="921"/>
+      <c r="D22" s="920" t="str">
         <f>D3</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E22" s="925"/>
-      <c r="F22" s="924" t="str">
+      <c r="E22" s="921"/>
+      <c r="F22" s="920" t="str">
         <f>F3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G22" s="925"/>
+      <c r="G22" s="921"/>
     </row>
     <row r="23" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="536"/>
@@ -10716,21 +10747,21 @@
       <c r="A41" s="538" t="s">
         <v>432</v>
       </c>
-      <c r="B41" s="914" t="str">
+      <c r="B41" s="910" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C41" s="915"/>
-      <c r="D41" s="916" t="str">
+      <c r="C41" s="911"/>
+      <c r="D41" s="912" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E41" s="917"/>
-      <c r="F41" s="916" t="str">
+      <c r="E41" s="913"/>
+      <c r="F41" s="912" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G41" s="917"/>
+      <c r="G41" s="913"/>
       <c r="N41" s="731"/>
       <c r="O41" s="758" t="s">
         <v>520</v>
@@ -10939,15 +10970,11 @@
         <v>445</v>
       </c>
       <c r="E53" s="734"/>
-      <c r="F53" s="935" t="s">
+      <c r="F53" s="931" t="s">
         <v>567</v>
       </c>
-      <c r="G53" s="913"/>
-      <c r="H53" s="913"/>
-      <c r="I53" s="734"/>
-      <c r="J53" s="734"/>
-      <c r="K53" s="734"/>
-      <c r="L53" s="734"/>
+      <c r="G53" s="909"/>
+      <c r="H53" s="909"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="727" t="s">
@@ -10957,10 +10984,6 @@
       <c r="C54" s="601"/>
       <c r="D54" s="737"/>
       <c r="E54" s="734"/>
-      <c r="I54" s="734"/>
-      <c r="J54" s="734"/>
-      <c r="K54" s="734"/>
-      <c r="L54" s="734"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="727" t="s">
@@ -11104,11 +11127,11 @@
         <v>445</v>
       </c>
       <c r="E63" s="734"/>
-      <c r="F63" s="935" t="s">
+      <c r="F63" s="931" t="s">
         <v>568</v>
       </c>
-      <c r="G63" s="913"/>
-      <c r="H63" s="913"/>
+      <c r="G63" s="909"/>
+      <c r="H63" s="909"/>
       <c r="I63" s="734"/>
       <c r="J63" s="734"/>
       <c r="K63" s="734"/>
@@ -11253,26 +11276,34 @@
       <c r="F72" s="735"/>
       <c r="G72" s="735"/>
       <c r="H72" s="735"/>
-      <c r="I72" s="735"/>
-      <c r="J72" s="735"/>
-      <c r="K72" s="735"/>
-      <c r="L72" s="735"/>
+      <c r="I72" s="734"/>
+      <c r="J72" s="734"/>
+      <c r="K72" s="734"/>
+      <c r="L72" s="734"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73" s="521" t="s">
         <v>446</v>
       </c>
+      <c r="I73" s="734"/>
+      <c r="J73" s="734"/>
+      <c r="K73" s="734"/>
+      <c r="L73" s="734"/>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74" s="644" t="s">
         <v>431</v>
       </c>
-      <c r="B74" s="913" t="s">
+      <c r="B74" s="909" t="s">
         <v>517</v>
       </c>
-      <c r="C74" s="913"/>
-      <c r="D74" s="913"/>
-      <c r="E74" s="913"/>
+      <c r="C74" s="909"/>
+      <c r="D74" s="909"/>
+      <c r="E74" s="909"/>
+      <c r="I74" s="735"/>
+      <c r="J74" s="735"/>
+      <c r="K74" s="735"/>
+      <c r="L74" s="735"/>
     </row>
     <row r="75" spans="1:19" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="549" t="s">
@@ -11293,9 +11324,6 @@
       <c r="H75" s="552" t="s">
         <v>448</v>
       </c>
-      <c r="I75" s="548"/>
-      <c r="J75" s="759"/>
-      <c r="K75" s="759"/>
     </row>
     <row r="76" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="526" t="s">
@@ -11326,11 +11354,6 @@
         <f>D3</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="I76" s="643" t="s">
-        <v>296</v>
-      </c>
-      <c r="J76" s="760"/>
-      <c r="K76" s="760"/>
     </row>
     <row r="77" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="638" t="s">
@@ -11343,9 +11366,9 @@
       <c r="F77" s="579"/>
       <c r="G77" s="617"/>
       <c r="H77" s="580"/>
-      <c r="I77" s="621"/>
-      <c r="J77" s="761"/>
-      <c r="K77" s="761"/>
+      <c r="I77" s="548"/>
+      <c r="J77" s="759"/>
+      <c r="K77" s="759"/>
       <c r="N77" s="744" t="s">
         <v>449</v>
       </c>
@@ -11360,7 +11383,7 @@
       <c r="Q77" s="745" t="s">
         <v>449</v>
       </c>
-      <c r="R77" s="765" t="str">
+      <c r="R77" s="763" t="str">
         <f>$D$3</f>
         <v>[#previous_year#]</v>
       </c>
@@ -11380,9 +11403,11 @@
       <c r="F78" s="581"/>
       <c r="G78" s="618"/>
       <c r="H78" s="582"/>
-      <c r="I78" s="622"/>
-      <c r="J78" s="761"/>
-      <c r="K78" s="761"/>
+      <c r="I78" s="643" t="s">
+        <v>296</v>
+      </c>
+      <c r="J78" s="760"/>
+      <c r="K78" s="760"/>
       <c r="N78" s="739" t="s">
         <v>450</v>
       </c>
@@ -11417,7 +11442,7 @@
       <c r="F79" s="581"/>
       <c r="G79" s="618"/>
       <c r="H79" s="582"/>
-      <c r="I79" s="622"/>
+      <c r="I79" s="621"/>
       <c r="J79" s="761"/>
       <c r="K79" s="761"/>
       <c r="N79" s="747" t="s">
@@ -11491,9 +11516,9 @@
       <c r="F81" s="583"/>
       <c r="G81" s="619"/>
       <c r="H81" s="584"/>
-      <c r="I81" s="623"/>
-      <c r="J81" s="762"/>
-      <c r="K81" s="762"/>
+      <c r="I81" s="622"/>
+      <c r="J81" s="761"/>
+      <c r="K81" s="761"/>
       <c r="N81" s="747" t="s">
         <v>453</v>
       </c>
@@ -11528,9 +11553,9 @@
       <c r="F82" s="585"/>
       <c r="G82" s="620"/>
       <c r="H82" s="586"/>
-      <c r="I82" s="624"/>
-      <c r="J82" s="762"/>
-      <c r="K82" s="762"/>
+      <c r="I82" s="622"/>
+      <c r="J82" s="761"/>
+      <c r="K82" s="761"/>
       <c r="N82" s="747" t="s">
         <v>454</v>
       </c>
@@ -11555,6 +11580,9 @@
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I83" s="623"/>
+      <c r="J83" s="762"/>
+      <c r="K83" s="762"/>
       <c r="N83" s="747" t="s">
         <v>456</v>
       </c>
@@ -11582,46 +11610,49 @@
       <c r="A84" s="555" t="s">
         <v>457</v>
       </c>
+      <c r="I84" s="624"/>
+      <c r="J84" s="762"/>
+      <c r="K84" s="762"/>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B85" s="928" t="str">
+      <c r="B85" s="924" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C85" s="929"/>
-      <c r="D85" s="928" t="str">
+      <c r="C85" s="925"/>
+      <c r="D85" s="924" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E85" s="929"/>
-      <c r="F85" s="928" t="str">
+      <c r="E85" s="925"/>
+      <c r="F85" s="924" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G85" s="929"/>
+      <c r="G85" s="925"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="522"/>
-      <c r="B86" s="873" t="s">
+      <c r="B86" s="869" t="s">
         <v>329</v>
       </c>
-      <c r="C86" s="874"/>
-      <c r="D86" s="873" t="s">
+      <c r="C86" s="870"/>
+      <c r="D86" s="869" t="s">
         <v>329</v>
       </c>
-      <c r="E86" s="874"/>
-      <c r="F86" s="873" t="s">
+      <c r="E86" s="870"/>
+      <c r="F86" s="869" t="s">
         <v>329</v>
       </c>
-      <c r="G86" s="874"/>
+      <c r="G86" s="870"/>
       <c r="N86" s="739" t="s">
         <v>458</v>
       </c>
-      <c r="O86" s="765" t="str">
+      <c r="O86" s="763" t="str">
         <f>F3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="P86" s="765" t="str">
+      <c r="P86" s="763" t="str">
         <f>D3</f>
         <v>[#previous_year#]</v>
       </c>
@@ -11894,36 +11925,36 @@
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B101" s="928" t="str">
+      <c r="B101" s="924" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C101" s="929"/>
-      <c r="D101" s="928" t="str">
+      <c r="C101" s="925"/>
+      <c r="D101" s="924" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E101" s="929"/>
-      <c r="F101" s="928" t="str">
+      <c r="E101" s="925"/>
+      <c r="F101" s="924" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G101" s="929"/>
+      <c r="G101" s="925"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="522"/>
-      <c r="B102" s="873" t="s">
+      <c r="B102" s="869" t="s">
         <v>329</v>
       </c>
-      <c r="C102" s="874"/>
-      <c r="D102" s="873" t="s">
+      <c r="C102" s="870"/>
+      <c r="D102" s="869" t="s">
         <v>329</v>
       </c>
-      <c r="E102" s="874"/>
-      <c r="F102" s="873" t="s">
+      <c r="E102" s="870"/>
+      <c r="F102" s="869" t="s">
         <v>329</v>
       </c>
-      <c r="G102" s="874"/>
+      <c r="G102" s="870"/>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" s="523" t="s">
@@ -11950,15 +11981,15 @@
       <c r="N103" s="739" t="s">
         <v>458</v>
       </c>
-      <c r="O103" s="765" t="str">
+      <c r="O103" s="763" t="str">
         <f>$F$3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="P103" s="765" t="str">
+      <c r="P103" s="763" t="str">
         <f>$D$3</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="Q103" s="765" t="str">
+      <c r="Q103" s="763" t="str">
         <f>$B$3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
@@ -12204,36 +12235,36 @@
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B116" s="930" t="str">
+      <c r="B116" s="926" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C116" s="931"/>
-      <c r="D116" s="930" t="str">
+      <c r="C116" s="927"/>
+      <c r="D116" s="926" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E116" s="931"/>
-      <c r="F116" s="930" t="str">
+      <c r="E116" s="927"/>
+      <c r="F116" s="926" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G116" s="931"/>
+      <c r="G116" s="927"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" s="561"/>
-      <c r="B117" s="932" t="s">
+      <c r="B117" s="928" t="s">
         <v>329</v>
       </c>
-      <c r="C117" s="933"/>
-      <c r="D117" s="932" t="s">
+      <c r="C117" s="929"/>
+      <c r="D117" s="928" t="s">
         <v>329</v>
       </c>
-      <c r="E117" s="933"/>
-      <c r="F117" s="932" t="s">
+      <c r="E117" s="929"/>
+      <c r="F117" s="928" t="s">
         <v>329</v>
       </c>
-      <c r="G117" s="933"/>
+      <c r="G117" s="929"/>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" s="562" t="s">
@@ -12257,21 +12288,18 @@
       <c r="G118" s="564" t="s">
         <v>110</v>
       </c>
-      <c r="I118" s="588"/>
-      <c r="J118" s="588"/>
-      <c r="K118" s="588"/>
       <c r="N118" s="739" t="s">
         <v>458</v>
       </c>
-      <c r="O118" s="765" t="str">
+      <c r="O118" s="763" t="str">
         <f>$F$3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="P118" s="765" t="str">
+      <c r="P118" s="763" t="str">
         <f>$D$3</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="Q118" s="765" t="str">
+      <c r="Q118" s="763" t="str">
         <f>$B$3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
@@ -12292,9 +12320,6 @@
         <v>100</v>
       </c>
       <c r="G119" s="587"/>
-      <c r="I119" s="588"/>
-      <c r="J119" s="588"/>
-      <c r="K119" s="588"/>
       <c r="N119" s="556" t="s">
         <v>459</v>
       </c>
@@ -12507,6 +12532,9 @@
       <c r="E126" s="539"/>
       <c r="F126" s="612"/>
       <c r="G126" s="603"/>
+      <c r="I126" s="588"/>
+      <c r="J126" s="588"/>
+      <c r="K126" s="588"/>
       <c r="N126" s="557" t="s">
         <v>466</v>
       </c>
@@ -12531,29 +12559,32 @@
       <c r="E127" s="539"/>
       <c r="F127" s="609"/>
       <c r="G127" s="603"/>
+      <c r="I127" s="588"/>
+      <c r="J127" s="588"/>
+      <c r="K127" s="588"/>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" s="565" t="s">
         <v>417</v>
       </c>
-      <c r="B129" s="926" t="str">
+      <c r="B129" s="922" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C129" s="927"/>
-      <c r="D129" s="927"/>
+      <c r="C129" s="923"/>
+      <c r="D129" s="923"/>
       <c r="N129" s="739" t="s">
         <v>458</v>
       </c>
-      <c r="O129" s="765" t="str">
+      <c r="O129" s="763" t="str">
         <f>$F$3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="P129" s="765" t="str">
+      <c r="P129" s="763" t="str">
         <f>$D$3</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="Q129" s="765" t="str">
+      <c r="Q129" s="763" t="str">
         <f>$B$3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
@@ -16817,66 +16848,66 @@
       <c r="AR3" s="8"/>
     </row>
     <row r="4" spans="1:44" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="768" t="s">
+      <c r="A4" s="764" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="769"/>
-      <c r="C4" s="769"/>
-      <c r="D4" s="769"/>
-      <c r="E4" s="770"/>
-      <c r="F4" s="770"/>
-      <c r="G4" s="770"/>
-      <c r="H4" s="770"/>
-      <c r="I4" s="770"/>
-      <c r="J4" s="770"/>
-      <c r="K4" s="770"/>
-      <c r="L4" s="770"/>
-      <c r="M4" s="770"/>
-      <c r="N4" s="770"/>
-      <c r="O4" s="770"/>
-      <c r="P4" s="770"/>
-      <c r="Q4" s="770"/>
-      <c r="R4" s="770"/>
-      <c r="S4" s="770"/>
-      <c r="T4" s="770"/>
-      <c r="U4" s="770"/>
-      <c r="V4" s="770"/>
-      <c r="W4" s="770"/>
-      <c r="X4" s="770"/>
-      <c r="Y4" s="770"/>
-      <c r="Z4" s="770"/>
-      <c r="AA4" s="770"/>
-      <c r="AB4" s="770"/>
-      <c r="AC4" s="770"/>
-      <c r="AD4" s="770"/>
-      <c r="AE4" s="770"/>
-      <c r="AF4" s="770"/>
-      <c r="AG4" s="770"/>
-      <c r="AH4" s="770"/>
-      <c r="AI4" s="770"/>
-      <c r="AJ4" s="770"/>
-      <c r="AK4" s="770"/>
-      <c r="AL4" s="770"/>
-      <c r="AM4" s="770"/>
-      <c r="AN4" s="770"/>
-      <c r="AO4" s="770"/>
-      <c r="AP4" s="770"/>
-      <c r="AQ4" s="771" t="s">
+      <c r="B4" s="765"/>
+      <c r="C4" s="765"/>
+      <c r="D4" s="765"/>
+      <c r="E4" s="766"/>
+      <c r="F4" s="766"/>
+      <c r="G4" s="766"/>
+      <c r="H4" s="766"/>
+      <c r="I4" s="766"/>
+      <c r="J4" s="766"/>
+      <c r="K4" s="766"/>
+      <c r="L4" s="766"/>
+      <c r="M4" s="766"/>
+      <c r="N4" s="766"/>
+      <c r="O4" s="766"/>
+      <c r="P4" s="766"/>
+      <c r="Q4" s="766"/>
+      <c r="R4" s="766"/>
+      <c r="S4" s="766"/>
+      <c r="T4" s="766"/>
+      <c r="U4" s="766"/>
+      <c r="V4" s="766"/>
+      <c r="W4" s="766"/>
+      <c r="X4" s="766"/>
+      <c r="Y4" s="766"/>
+      <c r="Z4" s="766"/>
+      <c r="AA4" s="766"/>
+      <c r="AB4" s="766"/>
+      <c r="AC4" s="766"/>
+      <c r="AD4" s="766"/>
+      <c r="AE4" s="766"/>
+      <c r="AF4" s="766"/>
+      <c r="AG4" s="766"/>
+      <c r="AH4" s="766"/>
+      <c r="AI4" s="766"/>
+      <c r="AJ4" s="766"/>
+      <c r="AK4" s="766"/>
+      <c r="AL4" s="766"/>
+      <c r="AM4" s="766"/>
+      <c r="AN4" s="766"/>
+      <c r="AO4" s="766"/>
+      <c r="AP4" s="766"/>
+      <c r="AQ4" s="767" t="s">
         <v>62</v>
       </c>
-      <c r="AR4" s="771"/>
+      <c r="AR4" s="767"/>
     </row>
     <row r="5" spans="1:44" s="8" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="772" t="s">
+      <c r="A5" s="768" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="772" t="s">
+      <c r="B5" s="768" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="772" t="s">
+      <c r="C5" s="768" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="772" t="s">
+      <c r="D5" s="768" t="s">
         <v>66</v>
       </c>
       <c r="E5" s="16" t="s">
@@ -16936,10 +16967,10 @@
       <c r="W5" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="X5" s="776" t="s">
+      <c r="X5" s="772" t="s">
         <v>86</v>
       </c>
-      <c r="Y5" s="776" t="s">
+      <c r="Y5" s="772" t="s">
         <v>87</v>
       </c>
       <c r="Z5" s="20" t="s">
@@ -16969,7 +17000,7 @@
       <c r="AH5" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="AI5" s="776" t="s">
+      <c r="AI5" s="772" t="s">
         <v>96</v>
       </c>
       <c r="AJ5" s="20" t="s">
@@ -16978,33 +17009,33 @@
       <c r="AK5" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="AL5" s="772" t="s">
+      <c r="AL5" s="768" t="s">
         <v>99</v>
       </c>
-      <c r="AM5" s="772" t="s">
+      <c r="AM5" s="768" t="s">
         <v>100</v>
       </c>
-      <c r="AN5" s="772" t="s">
+      <c r="AN5" s="768" t="s">
         <v>101</v>
       </c>
-      <c r="AO5" s="772" t="s">
+      <c r="AO5" s="768" t="s">
         <v>102</v>
       </c>
-      <c r="AP5" s="772" t="s">
+      <c r="AP5" s="768" t="s">
         <v>103</v>
       </c>
       <c r="AQ5" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="AR5" s="774" t="s">
+      <c r="AR5" s="770" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:44" s="11" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="773"/>
-      <c r="B6" s="773"/>
-      <c r="C6" s="773"/>
-      <c r="D6" s="773"/>
+      <c r="A6" s="769"/>
+      <c r="B6" s="769"/>
+      <c r="C6" s="769"/>
+      <c r="D6" s="769"/>
       <c r="E6" s="18" t="s">
         <v>106</v>
       </c>
@@ -17062,8 +17093,8 @@
       <c r="W6" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="X6" s="777"/>
-      <c r="Y6" s="777"/>
+      <c r="X6" s="773"/>
+      <c r="Y6" s="773"/>
       <c r="Z6" s="11" t="s">
         <v>107</v>
       </c>
@@ -17091,22 +17122,22 @@
       <c r="AH6" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="AI6" s="777"/>
+      <c r="AI6" s="773"/>
       <c r="AJ6" s="11" t="s">
         <v>107</v>
       </c>
       <c r="AK6" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="AL6" s="773"/>
-      <c r="AM6" s="773"/>
-      <c r="AN6" s="773"/>
-      <c r="AO6" s="773"/>
-      <c r="AP6" s="773"/>
+      <c r="AL6" s="769"/>
+      <c r="AM6" s="769"/>
+      <c r="AN6" s="769"/>
+      <c r="AO6" s="769"/>
+      <c r="AP6" s="769"/>
       <c r="AQ6" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="AR6" s="775"/>
+      <c r="AR6" s="771"/>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="AD7" s="10"/>
@@ -57180,10 +57211,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="778" t="s">
+      <c r="A1" s="774" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="780" t="s">
+      <c r="B1" s="776" t="s">
         <v>64</v>
       </c>
       <c r="C1" s="689" t="s">
@@ -57233,8 +57264,8 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="779"/>
-      <c r="B2" s="781"/>
+      <c r="A2" s="775"/>
+      <c r="B2" s="777"/>
       <c r="C2" s="11" t="s">
         <v>107</v>
       </c>
@@ -57397,123 +57428,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:95" s="680" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="782" t="s">
+      <c r="A1" s="778" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="783"/>
-      <c r="C1" s="783"/>
-      <c r="D1" s="783"/>
-      <c r="E1" s="783"/>
-      <c r="F1" s="783"/>
-      <c r="G1" s="783"/>
-      <c r="H1" s="784" t="s">
+      <c r="B1" s="779"/>
+      <c r="C1" s="779"/>
+      <c r="D1" s="779"/>
+      <c r="E1" s="779"/>
+      <c r="F1" s="779"/>
+      <c r="G1" s="779"/>
+      <c r="H1" s="780" t="s">
         <v>526</v>
       </c>
-      <c r="I1" s="785"/>
-      <c r="J1" s="785"/>
-      <c r="K1" s="785"/>
-      <c r="L1" s="785"/>
-      <c r="M1" s="786"/>
-      <c r="N1" s="787" t="s">
+      <c r="I1" s="781"/>
+      <c r="J1" s="781"/>
+      <c r="K1" s="781"/>
+      <c r="L1" s="781"/>
+      <c r="M1" s="782"/>
+      <c r="N1" s="783" t="s">
         <v>123</v>
       </c>
-      <c r="O1" s="788"/>
-      <c r="P1" s="788"/>
-      <c r="Q1" s="788"/>
-      <c r="R1" s="788"/>
-      <c r="S1" s="788"/>
-      <c r="T1" s="788"/>
-      <c r="U1" s="788"/>
-      <c r="V1" s="789" t="s">
+      <c r="O1" s="784"/>
+      <c r="P1" s="784"/>
+      <c r="Q1" s="784"/>
+      <c r="R1" s="784"/>
+      <c r="S1" s="784"/>
+      <c r="T1" s="784"/>
+      <c r="U1" s="784"/>
+      <c r="V1" s="785" t="s">
         <v>124</v>
       </c>
-      <c r="W1" s="790"/>
-      <c r="X1" s="791"/>
-      <c r="Y1" s="791"/>
-      <c r="Z1" s="792"/>
-      <c r="AA1" s="793" t="s">
+      <c r="W1" s="786"/>
+      <c r="X1" s="787"/>
+      <c r="Y1" s="787"/>
+      <c r="Z1" s="788"/>
+      <c r="AA1" s="789" t="s">
         <v>125</v>
       </c>
-      <c r="AB1" s="794"/>
-      <c r="AC1" s="794"/>
-      <c r="AD1" s="794"/>
-      <c r="AE1" s="794"/>
-      <c r="AF1" s="794"/>
-      <c r="AG1" s="794"/>
-      <c r="AH1" s="794"/>
-      <c r="AI1" s="794"/>
-      <c r="AJ1" s="794"/>
-      <c r="AK1" s="794"/>
-      <c r="AL1" s="794"/>
-      <c r="AM1" s="794"/>
+      <c r="AB1" s="790"/>
+      <c r="AC1" s="790"/>
+      <c r="AD1" s="790"/>
+      <c r="AE1" s="790"/>
+      <c r="AF1" s="790"/>
+      <c r="AG1" s="790"/>
+      <c r="AH1" s="790"/>
+      <c r="AI1" s="790"/>
+      <c r="AJ1" s="790"/>
+      <c r="AK1" s="790"/>
+      <c r="AL1" s="790"/>
+      <c r="AM1" s="790"/>
       <c r="AN1" s="56"/>
       <c r="AO1" s="57"/>
-      <c r="AP1" s="806" t="s">
+      <c r="AP1" s="802" t="s">
         <v>126</v>
       </c>
-      <c r="AQ1" s="788"/>
-      <c r="AR1" s="788"/>
-      <c r="AS1" s="788"/>
-      <c r="AT1" s="788"/>
-      <c r="AU1" s="788"/>
-      <c r="AV1" s="788"/>
-      <c r="AW1" s="807"/>
-      <c r="AX1" s="814" t="s">
+      <c r="AQ1" s="784"/>
+      <c r="AR1" s="784"/>
+      <c r="AS1" s="784"/>
+      <c r="AT1" s="784"/>
+      <c r="AU1" s="784"/>
+      <c r="AV1" s="784"/>
+      <c r="AW1" s="803"/>
+      <c r="AX1" s="810" t="s">
         <v>127</v>
       </c>
-      <c r="AY1" s="815"/>
-      <c r="AZ1" s="815"/>
-      <c r="BA1" s="815"/>
-      <c r="BB1" s="815"/>
-      <c r="BC1" s="816"/>
-      <c r="BD1" s="817" t="s">
+      <c r="AY1" s="811"/>
+      <c r="AZ1" s="811"/>
+      <c r="BA1" s="811"/>
+      <c r="BB1" s="811"/>
+      <c r="BC1" s="812"/>
+      <c r="BD1" s="813" t="s">
         <v>128</v>
       </c>
-      <c r="BE1" s="818"/>
-      <c r="BF1" s="818"/>
-      <c r="BG1" s="818"/>
-      <c r="BH1" s="818"/>
-      <c r="BI1" s="819"/>
-      <c r="BJ1" s="820" t="s">
+      <c r="BE1" s="814"/>
+      <c r="BF1" s="814"/>
+      <c r="BG1" s="814"/>
+      <c r="BH1" s="814"/>
+      <c r="BI1" s="815"/>
+      <c r="BJ1" s="816" t="s">
         <v>129</v>
       </c>
-      <c r="BK1" s="821"/>
-      <c r="BL1" s="821"/>
-      <c r="BM1" s="821"/>
-      <c r="BN1" s="821"/>
-      <c r="BO1" s="821"/>
-      <c r="BP1" s="822"/>
-      <c r="BQ1" s="795" t="s">
+      <c r="BK1" s="817"/>
+      <c r="BL1" s="817"/>
+      <c r="BM1" s="817"/>
+      <c r="BN1" s="817"/>
+      <c r="BO1" s="817"/>
+      <c r="BP1" s="818"/>
+      <c r="BQ1" s="791" t="s">
         <v>130</v>
       </c>
-      <c r="BR1" s="796"/>
-      <c r="BS1" s="796"/>
-      <c r="BT1" s="796"/>
-      <c r="BU1" s="796"/>
-      <c r="BV1" s="796"/>
+      <c r="BR1" s="792"/>
+      <c r="BS1" s="792"/>
+      <c r="BT1" s="792"/>
+      <c r="BU1" s="792"/>
+      <c r="BV1" s="792"/>
       <c r="BW1" s="57"/>
       <c r="BX1" s="58"/>
-      <c r="BY1" s="797" t="s">
+      <c r="BY1" s="793" t="s">
         <v>131</v>
       </c>
-      <c r="BZ1" s="798"/>
-      <c r="CA1" s="798"/>
-      <c r="CB1" s="798"/>
-      <c r="CC1" s="798"/>
-      <c r="CD1" s="798"/>
-      <c r="CE1" s="798"/>
-      <c r="CF1" s="799"/>
-      <c r="CG1" s="799"/>
-      <c r="CH1" s="799"/>
-      <c r="CI1" s="799"/>
-      <c r="CJ1" s="799"/>
-      <c r="CK1" s="799"/>
-      <c r="CL1" s="799"/>
-      <c r="CM1" s="799"/>
-      <c r="CN1" s="799"/>
-      <c r="CO1" s="799"/>
-      <c r="CP1" s="799"/>
-      <c r="CQ1" s="799"/>
+      <c r="BZ1" s="794"/>
+      <c r="CA1" s="794"/>
+      <c r="CB1" s="794"/>
+      <c r="CC1" s="794"/>
+      <c r="CD1" s="794"/>
+      <c r="CE1" s="794"/>
+      <c r="CF1" s="795"/>
+      <c r="CG1" s="795"/>
+      <c r="CH1" s="795"/>
+      <c r="CI1" s="795"/>
+      <c r="CJ1" s="795"/>
+      <c r="CK1" s="795"/>
+      <c r="CL1" s="795"/>
+      <c r="CM1" s="795"/>
+      <c r="CN1" s="795"/>
+      <c r="CO1" s="795"/>
+      <c r="CP1" s="795"/>
+      <c r="CQ1" s="795"/>
     </row>
     <row r="2" spans="1:95" s="680" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="59" t="s">
@@ -57537,18 +57568,18 @@
       <c r="G2" s="60" t="s">
         <v>138</v>
       </c>
-      <c r="H2" s="800" t="s">
+      <c r="H2" s="796" t="s">
         <v>527</v>
       </c>
-      <c r="I2" s="801"/>
-      <c r="J2" s="801" t="s">
+      <c r="I2" s="797"/>
+      <c r="J2" s="797" t="s">
         <v>139</v>
       </c>
-      <c r="K2" s="801"/>
-      <c r="L2" s="801" t="s">
+      <c r="K2" s="797"/>
+      <c r="L2" s="797" t="s">
         <v>140</v>
       </c>
-      <c r="M2" s="802"/>
+      <c r="M2" s="798"/>
       <c r="N2" s="61" t="s">
         <v>132</v>
       </c>
@@ -57657,36 +57688,36 @@
       <c r="AW2" s="63" t="s">
         <v>170</v>
       </c>
-      <c r="AX2" s="803" t="s">
+      <c r="AX2" s="799" t="s">
         <v>171</v>
       </c>
-      <c r="AY2" s="804"/>
-      <c r="AZ2" s="804"/>
-      <c r="BA2" s="804" t="s">
+      <c r="AY2" s="800"/>
+      <c r="AZ2" s="800"/>
+      <c r="BA2" s="800" t="s">
         <v>172</v>
       </c>
-      <c r="BB2" s="804"/>
-      <c r="BC2" s="805"/>
-      <c r="BD2" s="808" t="s">
+      <c r="BB2" s="800"/>
+      <c r="BC2" s="801"/>
+      <c r="BD2" s="804" t="s">
         <v>171</v>
       </c>
-      <c r="BE2" s="809"/>
-      <c r="BF2" s="809"/>
-      <c r="BG2" s="809" t="s">
+      <c r="BE2" s="805"/>
+      <c r="BF2" s="805"/>
+      <c r="BG2" s="805" t="s">
         <v>172</v>
       </c>
-      <c r="BH2" s="809"/>
-      <c r="BI2" s="810"/>
-      <c r="BJ2" s="811" t="s">
+      <c r="BH2" s="805"/>
+      <c r="BI2" s="806"/>
+      <c r="BJ2" s="807" t="s">
         <v>171</v>
       </c>
-      <c r="BK2" s="812"/>
-      <c r="BL2" s="812"/>
-      <c r="BM2" s="812" t="s">
+      <c r="BK2" s="808"/>
+      <c r="BL2" s="808"/>
+      <c r="BM2" s="808" t="s">
         <v>172</v>
       </c>
-      <c r="BN2" s="813"/>
-      <c r="BO2" s="813"/>
+      <c r="BN2" s="809"/>
+      <c r="BO2" s="809"/>
       <c r="BP2" s="73" t="s">
         <v>173</v>
       </c>
@@ -58421,127 +58452,127 @@
         <v>213</v>
       </c>
       <c r="L1" s="149"/>
-      <c r="M1" s="823" t="s">
+      <c r="M1" s="819" t="s">
         <v>214</v>
       </c>
-      <c r="N1" s="824" t="s">
+      <c r="N1" s="820" t="s">
         <v>215</v>
       </c>
-      <c r="O1" s="825"/>
-      <c r="P1" s="825"/>
-      <c r="Q1" s="825"/>
-      <c r="R1" s="826" t="s">
+      <c r="O1" s="821"/>
+      <c r="P1" s="821"/>
+      <c r="Q1" s="821"/>
+      <c r="R1" s="822" t="s">
         <v>526</v>
       </c>
-      <c r="S1" s="827"/>
-      <c r="T1" s="827"/>
-      <c r="U1" s="827"/>
-      <c r="V1" s="827"/>
-      <c r="W1" s="827"/>
-      <c r="X1" s="828"/>
-      <c r="Y1" s="829" t="s">
+      <c r="S1" s="823"/>
+      <c r="T1" s="823"/>
+      <c r="U1" s="823"/>
+      <c r="V1" s="823"/>
+      <c r="W1" s="823"/>
+      <c r="X1" s="824"/>
+      <c r="Y1" s="825" t="s">
         <v>534</v>
       </c>
-      <c r="Z1" s="818"/>
-      <c r="AA1" s="832" t="s">
+      <c r="Z1" s="814"/>
+      <c r="AA1" s="828" t="s">
         <v>216</v>
       </c>
-      <c r="AB1" s="843" t="s">
+      <c r="AB1" s="839" t="s">
         <v>217</v>
       </c>
-      <c r="AC1" s="839" t="s">
+      <c r="AC1" s="835" t="s">
         <v>218</v>
       </c>
-      <c r="AD1" s="840"/>
-      <c r="AE1" s="840"/>
-      <c r="AF1" s="841"/>
-      <c r="AG1" s="842" t="s">
+      <c r="AD1" s="836"/>
+      <c r="AE1" s="836"/>
+      <c r="AF1" s="837"/>
+      <c r="AG1" s="838" t="s">
         <v>219</v>
       </c>
-      <c r="AH1" s="827"/>
-      <c r="AI1" s="827"/>
-      <c r="AJ1" s="827"/>
-      <c r="AK1" s="827"/>
-      <c r="AL1" s="827"/>
-      <c r="AM1" s="827"/>
-      <c r="AN1" s="827"/>
-      <c r="AO1" s="843" t="s">
+      <c r="AH1" s="823"/>
+      <c r="AI1" s="823"/>
+      <c r="AJ1" s="823"/>
+      <c r="AK1" s="823"/>
+      <c r="AL1" s="823"/>
+      <c r="AM1" s="823"/>
+      <c r="AN1" s="823"/>
+      <c r="AO1" s="839" t="s">
         <v>220</v>
       </c>
-      <c r="AP1" s="829" t="s">
+      <c r="AP1" s="825" t="s">
         <v>533</v>
       </c>
-      <c r="AQ1" s="818"/>
-      <c r="AR1" s="818"/>
-      <c r="AS1" s="819"/>
-      <c r="AT1" s="846" t="s">
+      <c r="AQ1" s="814"/>
+      <c r="AR1" s="814"/>
+      <c r="AS1" s="815"/>
+      <c r="AT1" s="842" t="s">
         <v>221</v>
       </c>
-      <c r="AU1" s="847"/>
-      <c r="AV1" s="847"/>
-      <c r="AW1" s="847"/>
-      <c r="AX1" s="847"/>
-      <c r="AY1" s="847"/>
-      <c r="AZ1" s="847"/>
-      <c r="BA1" s="847"/>
-      <c r="BB1" s="847"/>
-      <c r="BC1" s="847"/>
-      <c r="BD1" s="847"/>
-      <c r="BE1" s="847"/>
-      <c r="BF1" s="847"/>
-      <c r="BG1" s="847"/>
-      <c r="BH1" s="847"/>
-      <c r="BI1" s="847"/>
-      <c r="BJ1" s="847"/>
-      <c r="BK1" s="847"/>
-      <c r="BL1" s="847"/>
-      <c r="BM1" s="847"/>
-      <c r="BN1" s="847"/>
-      <c r="BO1" s="847"/>
-      <c r="BP1" s="847"/>
-      <c r="BQ1" s="847"/>
-      <c r="BR1" s="847"/>
-      <c r="BS1" s="847"/>
-      <c r="BT1" s="847"/>
-      <c r="BU1" s="847"/>
-      <c r="BV1" s="847"/>
-      <c r="BW1" s="843" t="s">
+      <c r="AU1" s="843"/>
+      <c r="AV1" s="843"/>
+      <c r="AW1" s="843"/>
+      <c r="AX1" s="843"/>
+      <c r="AY1" s="843"/>
+      <c r="AZ1" s="843"/>
+      <c r="BA1" s="843"/>
+      <c r="BB1" s="843"/>
+      <c r="BC1" s="843"/>
+      <c r="BD1" s="843"/>
+      <c r="BE1" s="843"/>
+      <c r="BF1" s="843"/>
+      <c r="BG1" s="843"/>
+      <c r="BH1" s="843"/>
+      <c r="BI1" s="843"/>
+      <c r="BJ1" s="843"/>
+      <c r="BK1" s="843"/>
+      <c r="BL1" s="843"/>
+      <c r="BM1" s="843"/>
+      <c r="BN1" s="843"/>
+      <c r="BO1" s="843"/>
+      <c r="BP1" s="843"/>
+      <c r="BQ1" s="843"/>
+      <c r="BR1" s="843"/>
+      <c r="BS1" s="843"/>
+      <c r="BT1" s="843"/>
+      <c r="BU1" s="843"/>
+      <c r="BV1" s="843"/>
+      <c r="BW1" s="839" t="s">
         <v>222</v>
       </c>
-      <c r="BX1" s="829" t="s">
+      <c r="BX1" s="825" t="s">
         <v>532</v>
       </c>
-      <c r="BY1" s="818"/>
-      <c r="BZ1" s="818"/>
-      <c r="CA1" s="819"/>
-      <c r="CB1" s="855" t="s">
+      <c r="BY1" s="814"/>
+      <c r="BZ1" s="814"/>
+      <c r="CA1" s="815"/>
+      <c r="CB1" s="851" t="s">
         <v>554</v>
       </c>
-      <c r="CC1" s="837" t="s">
+      <c r="CC1" s="833" t="s">
         <v>125</v>
       </c>
-      <c r="CD1" s="837"/>
-      <c r="CE1" s="837"/>
-      <c r="CF1" s="837"/>
-      <c r="CG1" s="837"/>
-      <c r="CH1" s="837"/>
-      <c r="CI1" s="837"/>
-      <c r="CJ1" s="837"/>
-      <c r="CK1" s="837"/>
-      <c r="CL1" s="837"/>
-      <c r="CM1" s="837"/>
-      <c r="CN1" s="837"/>
+      <c r="CD1" s="833"/>
+      <c r="CE1" s="833"/>
+      <c r="CF1" s="833"/>
+      <c r="CG1" s="833"/>
+      <c r="CH1" s="833"/>
+      <c r="CI1" s="833"/>
+      <c r="CJ1" s="833"/>
+      <c r="CK1" s="833"/>
+      <c r="CL1" s="833"/>
+      <c r="CM1" s="833"/>
+      <c r="CN1" s="833"/>
       <c r="CO1" s="150"/>
-      <c r="CP1" s="851" t="s">
+      <c r="CP1" s="847" t="s">
         <v>130</v>
       </c>
-      <c r="CQ1" s="788"/>
-      <c r="CR1" s="788"/>
-      <c r="CS1" s="788"/>
-      <c r="CT1" s="788"/>
-      <c r="CU1" s="788"/>
-      <c r="CV1" s="788"/>
-      <c r="CW1" s="807"/>
+      <c r="CQ1" s="784"/>
+      <c r="CR1" s="784"/>
+      <c r="CS1" s="784"/>
+      <c r="CT1" s="784"/>
+      <c r="CU1" s="784"/>
+      <c r="CV1" s="784"/>
+      <c r="CW1" s="803"/>
     </row>
     <row r="2" spans="1:104" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="151" t="s">
@@ -58580,7 +58611,7 @@
       <c r="L2" s="155" t="s">
         <v>133</v>
       </c>
-      <c r="M2" s="823"/>
+      <c r="M2" s="819"/>
       <c r="N2" s="156" t="s">
         <v>227</v>
       </c>
@@ -58596,22 +58627,22 @@
       <c r="R2" s="161" t="s">
         <v>230</v>
       </c>
-      <c r="S2" s="834" t="s">
+      <c r="S2" s="830" t="s">
         <v>527</v>
       </c>
-      <c r="T2" s="813"/>
-      <c r="U2" s="835" t="s">
+      <c r="T2" s="809"/>
+      <c r="U2" s="831" t="s">
         <v>139</v>
       </c>
-      <c r="V2" s="835"/>
-      <c r="W2" s="835" t="s">
+      <c r="V2" s="831"/>
+      <c r="W2" s="831" t="s">
         <v>140</v>
       </c>
-      <c r="X2" s="836"/>
-      <c r="Y2" s="830"/>
-      <c r="Z2" s="831"/>
-      <c r="AA2" s="833"/>
-      <c r="AB2" s="844"/>
+      <c r="X2" s="832"/>
+      <c r="Y2" s="826"/>
+      <c r="Z2" s="827"/>
+      <c r="AA2" s="829"/>
+      <c r="AB2" s="840"/>
       <c r="AC2" s="157" t="s">
         <v>231</v>
       </c>
@@ -58624,81 +58655,81 @@
       <c r="AF2" s="157" t="s">
         <v>234</v>
       </c>
-      <c r="AG2" s="845" t="s">
+      <c r="AG2" s="841" t="s">
         <v>235</v>
       </c>
-      <c r="AH2" s="838"/>
-      <c r="AI2" s="838" t="s">
+      <c r="AH2" s="834"/>
+      <c r="AI2" s="834" t="s">
         <v>236</v>
       </c>
-      <c r="AJ2" s="838"/>
-      <c r="AK2" s="838" t="s">
+      <c r="AJ2" s="834"/>
+      <c r="AK2" s="834" t="s">
         <v>237</v>
       </c>
-      <c r="AL2" s="838"/>
+      <c r="AL2" s="834"/>
       <c r="AM2" s="158" t="s">
         <v>238</v>
       </c>
       <c r="AN2" s="158" t="s">
         <v>239</v>
       </c>
-      <c r="AO2" s="844"/>
-      <c r="AP2" s="830" t="s">
+      <c r="AO2" s="840"/>
+      <c r="AP2" s="826" t="s">
         <v>240</v>
       </c>
-      <c r="AQ2" s="831"/>
-      <c r="AR2" s="848" t="s">
+      <c r="AQ2" s="827"/>
+      <c r="AR2" s="844" t="s">
         <v>241</v>
       </c>
-      <c r="AS2" s="849"/>
-      <c r="AT2" s="838" t="s">
+      <c r="AS2" s="845"/>
+      <c r="AT2" s="834" t="s">
         <v>242</v>
       </c>
-      <c r="AU2" s="838"/>
-      <c r="AV2" s="850" t="s">
+      <c r="AU2" s="834"/>
+      <c r="AV2" s="846" t="s">
         <v>243</v>
       </c>
-      <c r="AW2" s="850"/>
-      <c r="AX2" s="850" t="s">
+      <c r="AW2" s="846"/>
+      <c r="AX2" s="846" t="s">
         <v>244</v>
       </c>
-      <c r="AY2" s="850"/>
+      <c r="AY2" s="846"/>
       <c r="AZ2" s="158" t="s">
         <v>245</v>
       </c>
       <c r="BA2" s="158" t="s">
         <v>246</v>
       </c>
-      <c r="BB2" s="838" t="s">
+      <c r="BB2" s="834" t="s">
         <v>247</v>
       </c>
-      <c r="BC2" s="838"/>
-      <c r="BD2" s="850" t="s">
+      <c r="BC2" s="834"/>
+      <c r="BD2" s="846" t="s">
         <v>248</v>
       </c>
-      <c r="BE2" s="850"/>
-      <c r="BF2" s="850" t="s">
+      <c r="BE2" s="846"/>
+      <c r="BF2" s="846" t="s">
         <v>249</v>
       </c>
-      <c r="BG2" s="850"/>
+      <c r="BG2" s="846"/>
       <c r="BH2" s="158" t="s">
         <v>250</v>
       </c>
       <c r="BI2" s="158" t="s">
         <v>251</v>
       </c>
-      <c r="BJ2" s="838" t="s">
+      <c r="BJ2" s="834" t="s">
         <v>252</v>
       </c>
-      <c r="BK2" s="838"/>
-      <c r="BL2" s="850" t="s">
+      <c r="BK2" s="834"/>
+      <c r="BL2" s="846" t="s">
         <v>253</v>
       </c>
-      <c r="BM2" s="850"/>
-      <c r="BN2" s="850" t="s">
+      <c r="BM2" s="846"/>
+      <c r="BN2" s="846" t="s">
         <v>254</v>
       </c>
-      <c r="BO2" s="850"/>
+      <c r="BO2" s="846"/>
       <c r="BP2" s="158" t="s">
         <v>255</v>
       </c>
@@ -58720,16 +58751,16 @@
       <c r="BV2" s="158" t="s">
         <v>261</v>
       </c>
-      <c r="BW2" s="844"/>
-      <c r="BX2" s="830" t="s">
+      <c r="BW2" s="840"/>
+      <c r="BX2" s="826" t="s">
         <v>240</v>
       </c>
-      <c r="BY2" s="831"/>
-      <c r="BZ2" s="848" t="s">
+      <c r="BY2" s="827"/>
+      <c r="BZ2" s="844" t="s">
         <v>241</v>
       </c>
-      <c r="CA2" s="849"/>
-      <c r="CB2" s="855"/>
+      <c r="CA2" s="845"/>
+      <c r="CB2" s="851"/>
       <c r="CC2" s="142" t="s">
         <v>150</v>
       </c>
@@ -58769,22 +58800,22 @@
       <c r="CO2" s="144" t="s">
         <v>536</v>
       </c>
-      <c r="CP2" s="854" t="s">
+      <c r="CP2" s="850" t="s">
         <v>263</v>
       </c>
-      <c r="CQ2" s="852"/>
-      <c r="CR2" s="852" t="s">
+      <c r="CQ2" s="848"/>
+      <c r="CR2" s="848" t="s">
         <v>264</v>
       </c>
-      <c r="CS2" s="852"/>
-      <c r="CT2" s="852" t="s">
+      <c r="CS2" s="848"/>
+      <c r="CT2" s="848" t="s">
         <v>265</v>
       </c>
-      <c r="CU2" s="852"/>
-      <c r="CV2" s="852" t="s">
+      <c r="CU2" s="848"/>
+      <c r="CV2" s="848" t="s">
         <v>266</v>
       </c>
-      <c r="CW2" s="853"/>
+      <c r="CW2" s="849"/>
     </row>
     <row r="3" spans="1:104" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="172"/>
@@ -59730,102 +59761,102 @@
       <c r="K1" s="148"/>
       <c r="L1" s="149"/>
       <c r="M1" s="720"/>
-      <c r="N1" s="824"/>
-      <c r="O1" s="825"/>
-      <c r="P1" s="825"/>
-      <c r="Q1" s="825"/>
-      <c r="R1" s="826"/>
-      <c r="S1" s="827"/>
-      <c r="T1" s="827"/>
-      <c r="U1" s="827"/>
-      <c r="V1" s="827"/>
-      <c r="W1" s="827"/>
-      <c r="X1" s="828"/>
-      <c r="Y1" s="829"/>
-      <c r="Z1" s="818"/>
+      <c r="N1" s="820"/>
+      <c r="O1" s="821"/>
+      <c r="P1" s="821"/>
+      <c r="Q1" s="821"/>
+      <c r="R1" s="822"/>
+      <c r="S1" s="823"/>
+      <c r="T1" s="823"/>
+      <c r="U1" s="823"/>
+      <c r="V1" s="823"/>
+      <c r="W1" s="823"/>
+      <c r="X1" s="824"/>
+      <c r="Y1" s="825"/>
+      <c r="Z1" s="814"/>
       <c r="AA1" s="721"/>
       <c r="AB1" s="719"/>
-      <c r="AC1" s="839"/>
-      <c r="AD1" s="840"/>
-      <c r="AE1" s="840"/>
-      <c r="AF1" s="841"/>
-      <c r="AG1" s="842"/>
-      <c r="AH1" s="827"/>
-      <c r="AI1" s="827"/>
-      <c r="AJ1" s="827"/>
-      <c r="AK1" s="827"/>
-      <c r="AL1" s="827"/>
-      <c r="AM1" s="827"/>
-      <c r="AN1" s="827"/>
+      <c r="AC1" s="835"/>
+      <c r="AD1" s="836"/>
+      <c r="AE1" s="836"/>
+      <c r="AF1" s="837"/>
+      <c r="AG1" s="838"/>
+      <c r="AH1" s="823"/>
+      <c r="AI1" s="823"/>
+      <c r="AJ1" s="823"/>
+      <c r="AK1" s="823"/>
+      <c r="AL1" s="823"/>
+      <c r="AM1" s="823"/>
+      <c r="AN1" s="823"/>
       <c r="AO1" s="719"/>
-      <c r="AP1" s="829"/>
-      <c r="AQ1" s="818"/>
-      <c r="AR1" s="818"/>
-      <c r="AS1" s="819"/>
-      <c r="AT1" s="846"/>
-      <c r="AU1" s="847"/>
-      <c r="AV1" s="847"/>
-      <c r="AW1" s="847"/>
-      <c r="AX1" s="847"/>
-      <c r="AY1" s="847"/>
-      <c r="AZ1" s="847"/>
-      <c r="BA1" s="847"/>
-      <c r="BB1" s="847"/>
-      <c r="BC1" s="847"/>
-      <c r="BD1" s="847"/>
-      <c r="BE1" s="847"/>
-      <c r="BF1" s="847"/>
-      <c r="BG1" s="847"/>
-      <c r="BH1" s="847"/>
-      <c r="BI1" s="847"/>
-      <c r="BJ1" s="847"/>
-      <c r="BK1" s="847"/>
-      <c r="BL1" s="847"/>
-      <c r="BM1" s="847"/>
-      <c r="BN1" s="847"/>
-      <c r="BO1" s="847"/>
-      <c r="BP1" s="847"/>
-      <c r="BQ1" s="847"/>
-      <c r="BR1" s="847"/>
-      <c r="BS1" s="847"/>
-      <c r="BT1" s="847"/>
-      <c r="BU1" s="847"/>
-      <c r="BV1" s="847"/>
+      <c r="AP1" s="825"/>
+      <c r="AQ1" s="814"/>
+      <c r="AR1" s="814"/>
+      <c r="AS1" s="815"/>
+      <c r="AT1" s="842"/>
+      <c r="AU1" s="843"/>
+      <c r="AV1" s="843"/>
+      <c r="AW1" s="843"/>
+      <c r="AX1" s="843"/>
+      <c r="AY1" s="843"/>
+      <c r="AZ1" s="843"/>
+      <c r="BA1" s="843"/>
+      <c r="BB1" s="843"/>
+      <c r="BC1" s="843"/>
+      <c r="BD1" s="843"/>
+      <c r="BE1" s="843"/>
+      <c r="BF1" s="843"/>
+      <c r="BG1" s="843"/>
+      <c r="BH1" s="843"/>
+      <c r="BI1" s="843"/>
+      <c r="BJ1" s="843"/>
+      <c r="BK1" s="843"/>
+      <c r="BL1" s="843"/>
+      <c r="BM1" s="843"/>
+      <c r="BN1" s="843"/>
+      <c r="BO1" s="843"/>
+      <c r="BP1" s="843"/>
+      <c r="BQ1" s="843"/>
+      <c r="BR1" s="843"/>
+      <c r="BS1" s="843"/>
+      <c r="BT1" s="843"/>
+      <c r="BU1" s="843"/>
+      <c r="BV1" s="843"/>
       <c r="BW1" s="719"/>
-      <c r="BX1" s="829"/>
-      <c r="BY1" s="818"/>
-      <c r="BZ1" s="818"/>
-      <c r="CA1" s="819"/>
-      <c r="CB1" s="837"/>
-      <c r="CC1" s="837"/>
-      <c r="CD1" s="837"/>
-      <c r="CE1" s="837"/>
-      <c r="CF1" s="837"/>
-      <c r="CG1" s="837"/>
-      <c r="CH1" s="837"/>
-      <c r="CI1" s="837"/>
-      <c r="CJ1" s="837"/>
-      <c r="CK1" s="837"/>
-      <c r="CL1" s="837"/>
-      <c r="CM1" s="837"/>
+      <c r="BX1" s="825"/>
+      <c r="BY1" s="814"/>
+      <c r="BZ1" s="814"/>
+      <c r="CA1" s="815"/>
+      <c r="CB1" s="833"/>
+      <c r="CC1" s="833"/>
+      <c r="CD1" s="833"/>
+      <c r="CE1" s="833"/>
+      <c r="CF1" s="833"/>
+      <c r="CG1" s="833"/>
+      <c r="CH1" s="833"/>
+      <c r="CI1" s="833"/>
+      <c r="CJ1" s="833"/>
+      <c r="CK1" s="833"/>
+      <c r="CL1" s="833"/>
+      <c r="CM1" s="833"/>
       <c r="CN1" s="718"/>
-      <c r="CO1" s="851"/>
-      <c r="CP1" s="788"/>
-      <c r="CQ1" s="788"/>
-      <c r="CR1" s="788"/>
-      <c r="CS1" s="788"/>
-      <c r="CT1" s="788"/>
-      <c r="CU1" s="788"/>
-      <c r="CV1" s="807"/>
-      <c r="CW1" s="856"/>
-      <c r="CX1" s="857"/>
-      <c r="CY1" s="857"/>
-      <c r="CZ1" s="858"/>
-      <c r="DA1" s="857"/>
-      <c r="DB1" s="857"/>
-      <c r="DC1" s="858"/>
-      <c r="DD1" s="857"/>
-      <c r="DE1" s="857"/>
+      <c r="CO1" s="847"/>
+      <c r="CP1" s="784"/>
+      <c r="CQ1" s="784"/>
+      <c r="CR1" s="784"/>
+      <c r="CS1" s="784"/>
+      <c r="CT1" s="784"/>
+      <c r="CU1" s="784"/>
+      <c r="CV1" s="803"/>
+      <c r="CW1" s="852"/>
+      <c r="CX1" s="853"/>
+      <c r="CY1" s="853"/>
+      <c r="CZ1" s="854"/>
+      <c r="DA1" s="853"/>
+      <c r="DB1" s="853"/>
+      <c r="DC1" s="854"/>
+      <c r="DD1" s="853"/>
+      <c r="DE1" s="853"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -59864,12 +59895,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="861" t="s">
+      <c r="A1" s="857" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="862"/>
-      <c r="C1" s="862"/>
-      <c r="D1" s="859" t="s">
+      <c r="B1" s="858"/>
+      <c r="C1" s="858"/>
+      <c r="D1" s="855" t="s">
         <v>269</v>
       </c>
     </row>
@@ -59883,7 +59914,7 @@
       <c r="C2" s="481" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="860"/>
+      <c r="D2" s="856"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="472"/>
@@ -59971,10 +60002,10 @@
       <c r="B2" s="207" t="s">
         <v>286</v>
       </c>
-      <c r="C2" s="863" t="s">
+      <c r="C2" s="859" t="s">
         <v>287</v>
       </c>
-      <c r="D2" s="863"/>
+      <c r="D2" s="859"/>
       <c r="E2" s="205"/>
       <c r="F2" s="205"/>
       <c r="G2" s="205"/>
@@ -60099,32 +60130,32 @@
     </row>
     <row r="7" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="204"/>
-      <c r="B7" s="864" t="s">
+      <c r="B7" s="860" t="s">
         <v>510</v>
       </c>
-      <c r="C7" s="864"/>
-      <c r="D7" s="864"/>
+      <c r="C7" s="860"/>
+      <c r="D7" s="860"/>
       <c r="E7" s="205"/>
       <c r="F7" s="205"/>
       <c r="G7" s="205"/>
       <c r="H7" s="205"/>
       <c r="I7" s="205"/>
-      <c r="J7" s="864" t="s">
+      <c r="J7" s="860" t="s">
         <v>509</v>
       </c>
-      <c r="K7" s="864"/>
-      <c r="L7" s="864"/>
+      <c r="K7" s="860"/>
+      <c r="L7" s="860"/>
       <c r="M7" s="205"/>
       <c r="N7" s="205"/>
       <c r="O7" s="205"/>
       <c r="P7" s="206" t="s">
         <v>291</v>
       </c>
-      <c r="Q7" s="864" t="s">
+      <c r="Q7" s="860" t="s">
         <v>510</v>
       </c>
-      <c r="R7" s="864"/>
-      <c r="S7" s="864"/>
+      <c r="R7" s="860"/>
+      <c r="S7" s="860"/>
       <c r="T7" s="205"/>
       <c r="U7" s="219" t="s">
         <v>292</v>
@@ -60158,41 +60189,41 @@
       <c r="B9" s="220" t="s">
         <v>512</v>
       </c>
-      <c r="C9" s="865" t="s">
+      <c r="C9" s="861" t="s">
         <v>293</v>
       </c>
-      <c r="D9" s="866"/>
-      <c r="E9" s="865" t="s">
+      <c r="D9" s="862"/>
+      <c r="E9" s="861" t="s">
         <v>294</v>
       </c>
-      <c r="F9" s="866"/>
+      <c r="F9" s="862"/>
       <c r="G9" s="205"/>
       <c r="H9" s="205"/>
       <c r="I9" s="205"/>
       <c r="J9" s="220" t="s">
         <v>512</v>
       </c>
-      <c r="K9" s="865" t="s">
+      <c r="K9" s="861" t="s">
         <v>293</v>
       </c>
-      <c r="L9" s="866"/>
-      <c r="M9" s="865" t="s">
+      <c r="L9" s="862"/>
+      <c r="M9" s="861" t="s">
         <v>294</v>
       </c>
-      <c r="N9" s="866"/>
+      <c r="N9" s="862"/>
       <c r="O9" s="205"/>
       <c r="P9" s="205"/>
       <c r="Q9" s="220" t="s">
         <v>512</v>
       </c>
-      <c r="R9" s="865" t="s">
+      <c r="R9" s="861" t="s">
         <v>293</v>
       </c>
-      <c r="S9" s="866"/>
-      <c r="T9" s="865" t="s">
+      <c r="S9" s="862"/>
+      <c r="T9" s="861" t="s">
         <v>294</v>
       </c>
-      <c r="U9" s="866"/>
+      <c r="U9" s="862"/>
     </row>
     <row r="10" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="204"/>
@@ -60254,10 +60285,10 @@
       </c>
       <c r="C11" s="225"/>
       <c r="D11" s="225"/>
-      <c r="E11" s="867" t="s">
+      <c r="E11" s="863" t="s">
         <v>298</v>
       </c>
-      <c r="F11" s="868"/>
+      <c r="F11" s="864"/>
       <c r="G11" s="226"/>
       <c r="H11" s="226"/>
       <c r="I11" s="226"/>
@@ -60266,10 +60297,10 @@
       </c>
       <c r="K11" s="205"/>
       <c r="L11" s="205"/>
-      <c r="M11" s="870" t="s">
+      <c r="M11" s="866" t="s">
         <v>298</v>
       </c>
-      <c r="N11" s="871"/>
+      <c r="N11" s="867"/>
       <c r="O11" s="226"/>
       <c r="P11" s="226"/>
       <c r="Q11" s="224" t="s">
@@ -60277,10 +60308,10 @@
       </c>
       <c r="R11" s="225"/>
       <c r="S11" s="225"/>
-      <c r="T11" s="867" t="s">
+      <c r="T11" s="863" t="s">
         <v>298</v>
       </c>
-      <c r="U11" s="868"/>
+      <c r="U11" s="864"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="204"/>
@@ -60515,10 +60546,10 @@
       </c>
       <c r="C20" s="306"/>
       <c r="D20" s="253"/>
-      <c r="E20" s="867" t="s">
+      <c r="E20" s="863" t="s">
         <v>305</v>
       </c>
-      <c r="F20" s="868"/>
+      <c r="F20" s="864"/>
       <c r="G20" s="234"/>
       <c r="H20" s="234"/>
       <c r="I20" s="205"/>
@@ -60527,10 +60558,10 @@
       </c>
       <c r="K20" s="306"/>
       <c r="L20" s="253"/>
-      <c r="M20" s="867" t="s">
+      <c r="M20" s="863" t="s">
         <v>305</v>
       </c>
-      <c r="N20" s="868"/>
+      <c r="N20" s="864"/>
       <c r="O20" s="244"/>
       <c r="P20" s="244"/>
       <c r="Q20" s="224" t="s">
@@ -60538,10 +60569,10 @@
       </c>
       <c r="R20" s="306"/>
       <c r="S20" s="253"/>
-      <c r="T20" s="867" t="s">
+      <c r="T20" s="863" t="s">
         <v>305</v>
       </c>
-      <c r="U20" s="868"/>
+      <c r="U20" s="864"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="204"/>
@@ -60805,10 +60836,10 @@
       </c>
       <c r="C30" s="306"/>
       <c r="D30" s="253"/>
-      <c r="E30" s="867" t="s">
+      <c r="E30" s="863" t="s">
         <v>305</v>
       </c>
-      <c r="F30" s="868"/>
+      <c r="F30" s="864"/>
       <c r="G30" s="234"/>
       <c r="H30" s="234"/>
       <c r="I30" s="205"/>
@@ -60817,10 +60848,10 @@
       </c>
       <c r="K30" s="306"/>
       <c r="L30" s="253"/>
-      <c r="M30" s="867" t="s">
+      <c r="M30" s="863" t="s">
         <v>305</v>
       </c>
-      <c r="N30" s="868"/>
+      <c r="N30" s="864"/>
       <c r="O30" s="244"/>
       <c r="P30" s="244"/>
       <c r="Q30" s="224" t="s">
@@ -60828,10 +60859,10 @@
       </c>
       <c r="R30" s="306"/>
       <c r="S30" s="253"/>
-      <c r="T30" s="867" t="s">
+      <c r="T30" s="863" t="s">
         <v>305</v>
       </c>
-      <c r="U30" s="868"/>
+      <c r="U30" s="864"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" s="266"/>
@@ -61154,11 +61185,11 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="204"/>
-      <c r="B42" s="869"/>
-      <c r="C42" s="869"/>
-      <c r="D42" s="869"/>
-      <c r="E42" s="869"/>
-      <c r="F42" s="869"/>
+      <c r="B42" s="865"/>
+      <c r="C42" s="865"/>
+      <c r="D42" s="865"/>
+      <c r="E42" s="865"/>
+      <c r="F42" s="865"/>
       <c r="G42" s="244"/>
       <c r="H42" s="205"/>
       <c r="I42" s="244"/>
@@ -61353,8 +61384,8 @@
       <c r="B3" s="332" t="s">
         <v>286</v>
       </c>
-      <c r="C3" s="872"/>
-      <c r="D3" s="872"/>
+      <c r="C3" s="868"/>
+      <c r="D3" s="868"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C4" s="333"/>
@@ -61387,10 +61418,10 @@
       <c r="D10" s="340" t="s">
         <v>328</v>
       </c>
-      <c r="E10" s="873" t="s">
+      <c r="E10" s="869" t="s">
         <v>329</v>
       </c>
-      <c r="F10" s="874"/>
+      <c r="F10" s="870"/>
     </row>
     <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="341" t="s">
@@ -61541,10 +61572,10 @@
       <c r="D30" s="351" t="s">
         <v>328</v>
       </c>
-      <c r="E30" s="873" t="s">
+      <c r="E30" s="869" t="s">
         <v>329</v>
       </c>
-      <c r="F30" s="874"/>
+      <c r="F30" s="870"/>
     </row>
     <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="341" t="s">
@@ -61692,10 +61723,10 @@
       <c r="D49" s="351" t="s">
         <v>328</v>
       </c>
-      <c r="E49" s="873" t="s">
+      <c r="E49" s="869" t="s">
         <v>329</v>
       </c>
-      <c r="F49" s="874"/>
+      <c r="F49" s="870"/>
     </row>
     <row r="50" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="341" t="s">

</xml_diff>

<commit_message>
add column in register graph sheet
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20201216.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20201216.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="480" windowWidth="13740" windowHeight="7368" firstSheet="13" activeTab="19"/>
+    <workbookView xWindow="660" yWindow="480" windowWidth="13740" windowHeight="7368" firstSheet="15" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="576">
   <si>
     <t>Acronym</t>
   </si>
@@ -2182,10 +2182,6 @@
 Load in population equivalent (p.e.)</t>
   </si>
   <si>
-    <t>Comparison of compliance between [#previous_year_n2#], [#previous_year#] and [#current_year#] reporting
-Number of agglomerations</t>
-  </si>
-  <si>
     <t>Number of agglomerations</t>
   </si>
   <si>
@@ -2218,6 +2214,16 @@
   </si>
   <si>
     <t>Size of treatment plant  under the previous reporting</t>
+  </si>
+  <si>
+    <t>Not relevant (Pending Deadline)</t>
+  </si>
+  <si>
+    <t>Not relevant (other)</t>
+  </si>
+  <si>
+    <t>Comparison of compliance between [#previous_year_n2#], [#previous_year#] and [#current_year#] reporting
+Number of agglomerations</t>
   </si>
 </sst>
 </file>
@@ -5423,6 +5429,42 @@
     <xf numFmtId="0" fontId="10" fillId="46" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="45" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="43" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="40" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="39" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="38" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="41" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="44" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="42" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="47" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="46" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="31" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5511,6 +5553,45 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5547,9 +5628,6 @@
     <xf numFmtId="3" fontId="6" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5598,141 +5676,105 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5754,6 +5796,18 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -5763,23 +5817,11 @@
     <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -5809,6 +5851,39 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -5836,40 +5911,10 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5894,8 +5939,59 @@
     <xf numFmtId="3" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5907,107 +6003,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="45" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="43" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="40" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="39" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="38" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="41" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="44" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="42" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="47" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="46" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="31" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6639,8 +6645,8 @@
       <c r="B3" s="330" t="s">
         <v>280</v>
       </c>
-      <c r="C3" s="898"/>
-      <c r="D3" s="898"/>
+      <c r="C3" s="910"/>
+      <c r="D3" s="910"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C4" s="331"/>
@@ -6673,10 +6679,10 @@
       <c r="D10" s="338" t="s">
         <v>322</v>
       </c>
-      <c r="E10" s="899" t="s">
+      <c r="E10" s="911" t="s">
         <v>323</v>
       </c>
-      <c r="F10" s="900"/>
+      <c r="F10" s="912"/>
     </row>
     <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="339" t="s">
@@ -6827,10 +6833,10 @@
       <c r="D30" s="349" t="s">
         <v>322</v>
       </c>
-      <c r="E30" s="899" t="s">
+      <c r="E30" s="911" t="s">
         <v>323</v>
       </c>
-      <c r="F30" s="900"/>
+      <c r="F30" s="912"/>
     </row>
     <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="339" t="s">
@@ -6978,10 +6984,10 @@
       <c r="D49" s="349" t="s">
         <v>322</v>
       </c>
-      <c r="E49" s="899" t="s">
+      <c r="E49" s="911" t="s">
         <v>323</v>
       </c>
-      <c r="F49" s="900"/>
+      <c r="F49" s="912"/>
     </row>
     <row r="50" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="339" t="s">
@@ -7150,8 +7156,8 @@
       </c>
       <c r="C2" s="390"/>
       <c r="D2" s="390"/>
-      <c r="E2" s="896"/>
-      <c r="F2" s="896"/>
+      <c r="E2" s="901"/>
+      <c r="F2" s="901"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="389"/>
@@ -7183,13 +7189,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="387"/>
-      <c r="B6" s="897" t="s">
+      <c r="B6" s="902" t="s">
         <v>508</v>
       </c>
-      <c r="C6" s="897"/>
-      <c r="D6" s="897"/>
-      <c r="E6" s="897"/>
-      <c r="F6" s="897"/>
+      <c r="C6" s="902"/>
+      <c r="D6" s="902"/>
+      <c r="E6" s="902"/>
+      <c r="F6" s="902"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="387"/>
@@ -7204,14 +7210,14 @@
       <c r="B8" s="416" t="s">
         <v>545</v>
       </c>
-      <c r="C8" s="901" t="s">
+      <c r="C8" s="913" t="s">
         <v>287</v>
       </c>
-      <c r="D8" s="902"/>
-      <c r="E8" s="901" t="s">
+      <c r="D8" s="914"/>
+      <c r="E8" s="913" t="s">
         <v>288</v>
       </c>
-      <c r="F8" s="902"/>
+      <c r="F8" s="914"/>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="387"/>
@@ -7347,11 +7353,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="387"/>
-      <c r="B22" s="891"/>
-      <c r="C22" s="891"/>
-      <c r="D22" s="891"/>
-      <c r="E22" s="891"/>
-      <c r="F22" s="891"/>
+      <c r="B22" s="907"/>
+      <c r="C22" s="907"/>
+      <c r="D22" s="907"/>
+      <c r="E22" s="907"/>
+      <c r="F22" s="907"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="387"/>
@@ -7422,13 +7428,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="903" t="s">
+      <c r="B2" s="915" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="904" t="s">
+      <c r="C2" s="916" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="904" t="s">
+      <c r="D2" s="916" t="s">
         <v>219</v>
       </c>
       <c r="E2" s="441" t="s">
@@ -7463,9 +7469,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="903"/>
-      <c r="C3" s="905"/>
-      <c r="D3" s="905"/>
+      <c r="B3" s="915"/>
+      <c r="C3" s="917"/>
+      <c r="D3" s="917"/>
       <c r="E3" s="456" t="s">
         <v>349</v>
       </c>
@@ -7498,7 +7504,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="906" t="s">
+      <c r="B4" s="918" t="s">
         <v>352</v>
       </c>
       <c r="C4" s="442" t="s">
@@ -7517,7 +7523,7 @@
       <c r="N4" s="444"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="906"/>
+      <c r="B5" s="918"/>
       <c r="C5" s="442" t="s">
         <v>129</v>
       </c>
@@ -7534,7 +7540,7 @@
       <c r="N5" s="444"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="907"/>
+      <c r="B6" s="919"/>
       <c r="C6" s="452" t="s">
         <v>342</v>
       </c>
@@ -7648,43 +7654,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="920" t="s">
+      <c r="A1" s="923" t="s">
         <v>207</v>
       </c>
-      <c r="B1" s="921"/>
+      <c r="B1" s="924"/>
       <c r="C1" s="472"/>
-      <c r="D1" s="911" t="s">
+      <c r="D1" s="934" t="s">
         <v>354</v>
       </c>
-      <c r="E1" s="912"/>
-      <c r="F1" s="912"/>
-      <c r="G1" s="912"/>
-      <c r="H1" s="912"/>
-      <c r="I1" s="913"/>
-      <c r="J1" s="922" t="s">
+      <c r="E1" s="935"/>
+      <c r="F1" s="935"/>
+      <c r="G1" s="935"/>
+      <c r="H1" s="935"/>
+      <c r="I1" s="936"/>
+      <c r="J1" s="925" t="s">
         <v>355</v>
       </c>
-      <c r="K1" s="923"/>
-      <c r="L1" s="923"/>
-      <c r="M1" s="923"/>
-      <c r="N1" s="924"/>
-      <c r="O1" s="925" t="s">
+      <c r="K1" s="926"/>
+      <c r="L1" s="926"/>
+      <c r="M1" s="926"/>
+      <c r="N1" s="927"/>
+      <c r="O1" s="928" t="s">
         <v>356</v>
       </c>
-      <c r="P1" s="926"/>
-      <c r="Q1" s="927"/>
+      <c r="P1" s="929"/>
+      <c r="Q1" s="930"/>
       <c r="R1" s="459" t="s">
         <v>116</v>
       </c>
       <c r="S1" s="460"/>
-      <c r="T1" s="919" t="s">
+      <c r="T1" s="922" t="s">
         <v>556</v>
       </c>
-      <c r="U1" s="919"/>
-      <c r="V1" s="919"/>
-      <c r="W1" s="919"/>
-      <c r="X1" s="919"/>
-      <c r="Y1" s="919"/>
+      <c r="U1" s="922"/>
+      <c r="V1" s="922"/>
+      <c r="W1" s="922"/>
+      <c r="X1" s="922"/>
+      <c r="Y1" s="922"/>
     </row>
     <row r="2" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="462" t="s">
@@ -7696,18 +7702,18 @@
       <c r="C2" s="463" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="916" t="s">
+      <c r="D2" s="939" t="s">
         <v>358</v>
       </c>
-      <c r="E2" s="915"/>
-      <c r="F2" s="915" t="s">
+      <c r="E2" s="938"/>
+      <c r="F2" s="938" t="s">
         <v>359</v>
       </c>
-      <c r="G2" s="915"/>
-      <c r="H2" s="914" t="s">
+      <c r="G2" s="938"/>
+      <c r="H2" s="937" t="s">
         <v>360</v>
       </c>
-      <c r="I2" s="914"/>
+      <c r="I2" s="937"/>
       <c r="J2" s="464">
         <v>0</v>
       </c>
@@ -7738,18 +7744,18 @@
       <c r="S2" s="704" t="s">
         <v>127</v>
       </c>
-      <c r="T2" s="917" t="s">
+      <c r="T2" s="920" t="s">
         <v>520</v>
       </c>
-      <c r="U2" s="917"/>
-      <c r="V2" s="918" t="s">
+      <c r="U2" s="920"/>
+      <c r="V2" s="921" t="s">
         <v>542</v>
       </c>
-      <c r="W2" s="918"/>
-      <c r="X2" s="918" t="s">
+      <c r="W2" s="921"/>
+      <c r="X2" s="921" t="s">
         <v>543</v>
       </c>
-      <c r="Y2" s="918"/>
+      <c r="Y2" s="921"/>
     </row>
     <row r="3" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="467"/>
@@ -7775,13 +7781,13 @@
       <c r="I3" s="688" t="s">
         <v>105</v>
       </c>
-      <c r="J3" s="908" t="s">
+      <c r="J3" s="931" t="s">
         <v>365</v>
       </c>
-      <c r="K3" s="909"/>
-      <c r="L3" s="909"/>
-      <c r="M3" s="909"/>
-      <c r="N3" s="910"/>
+      <c r="K3" s="932"/>
+      <c r="L3" s="932"/>
+      <c r="M3" s="932"/>
+      <c r="N3" s="933"/>
       <c r="O3" s="475"/>
       <c r="P3" s="475"/>
       <c r="Q3" s="475"/>
@@ -9010,6 +9016,11 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:X4"/>
   <mergeCells count="12">
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D2:E2"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
@@ -9017,11 +9028,6 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9061,25 +9067,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="837" t="s">
+      <c r="A1" s="820" t="s">
         <v>366</v>
       </c>
-      <c r="B1" s="838"/>
-      <c r="C1" s="838"/>
-      <c r="D1" s="838"/>
-      <c r="E1" s="838"/>
-      <c r="F1" s="838"/>
+      <c r="B1" s="821"/>
+      <c r="C1" s="821"/>
+      <c r="D1" s="821"/>
+      <c r="E1" s="821"/>
+      <c r="F1" s="821"/>
       <c r="G1" s="489"/>
-      <c r="H1" s="933" t="s">
+      <c r="H1" s="946" t="s">
         <v>210</v>
       </c>
-      <c r="I1" s="934"/>
-      <c r="J1" s="934"/>
+      <c r="I1" s="947"/>
+      <c r="J1" s="947"/>
       <c r="K1" s="491"/>
       <c r="L1" s="481"/>
       <c r="M1" s="491"/>
       <c r="N1" s="482"/>
-      <c r="O1" s="931" t="s">
+      <c r="O1" s="944" t="s">
         <v>367</v>
       </c>
       <c r="P1" s="483"/>
@@ -9091,26 +9097,26 @@
       <c r="T1" s="481"/>
       <c r="U1" s="491"/>
       <c r="V1" s="482"/>
-      <c r="W1" s="931" t="s">
+      <c r="W1" s="944" t="s">
         <v>369</v>
       </c>
       <c r="X1" s="483"/>
-      <c r="Y1" s="935" t="s">
+      <c r="Y1" s="948" t="s">
         <v>370</v>
       </c>
-      <c r="Z1" s="935"/>
-      <c r="AA1" s="935"/>
-      <c r="AB1" s="935"/>
-      <c r="AC1" s="935"/>
-      <c r="AD1" s="936"/>
-      <c r="AE1" s="931" t="s">
+      <c r="Z1" s="948"/>
+      <c r="AA1" s="948"/>
+      <c r="AB1" s="948"/>
+      <c r="AC1" s="948"/>
+      <c r="AD1" s="949"/>
+      <c r="AE1" s="944" t="s">
         <v>371</v>
       </c>
-      <c r="AF1" s="930" t="s">
+      <c r="AF1" s="943" t="s">
         <v>541</v>
       </c>
-      <c r="AG1" s="919"/>
-      <c r="AH1" s="919"/>
+      <c r="AG1" s="922"/>
+      <c r="AH1" s="922"/>
       <c r="AI1" s="711"/>
       <c r="AJ1" s="711"/>
       <c r="AK1" s="711"/>
@@ -9169,56 +9175,56 @@
       <c r="C2" s="490" t="s">
         <v>373</v>
       </c>
-      <c r="D2" s="929" t="s">
+      <c r="D2" s="942" t="s">
         <v>546</v>
       </c>
-      <c r="E2" s="929"/>
-      <c r="F2" s="929" t="s">
+      <c r="E2" s="942"/>
+      <c r="F2" s="942" t="s">
         <v>547</v>
       </c>
-      <c r="G2" s="929"/>
+      <c r="G2" s="942"/>
       <c r="H2" s="485"/>
-      <c r="I2" s="928" t="s">
+      <c r="I2" s="940" t="s">
         <v>229</v>
       </c>
-      <c r="J2" s="928"/>
-      <c r="K2" s="928" t="s">
+      <c r="J2" s="940"/>
+      <c r="K2" s="940" t="s">
         <v>230</v>
       </c>
-      <c r="L2" s="928"/>
-      <c r="M2" s="928" t="s">
+      <c r="L2" s="940"/>
+      <c r="M2" s="940" t="s">
         <v>231</v>
       </c>
-      <c r="N2" s="937"/>
-      <c r="O2" s="932"/>
+      <c r="N2" s="941"/>
+      <c r="O2" s="945"/>
       <c r="P2" s="486"/>
-      <c r="Q2" s="928" t="s">
+      <c r="Q2" s="940" t="s">
         <v>229</v>
       </c>
-      <c r="R2" s="928"/>
-      <c r="S2" s="928" t="s">
+      <c r="R2" s="940"/>
+      <c r="S2" s="940" t="s">
         <v>230</v>
       </c>
-      <c r="T2" s="928"/>
-      <c r="U2" s="928" t="s">
+      <c r="T2" s="940"/>
+      <c r="U2" s="940" t="s">
         <v>231</v>
       </c>
-      <c r="V2" s="937"/>
-      <c r="W2" s="932"/>
+      <c r="V2" s="941"/>
+      <c r="W2" s="945"/>
       <c r="X2" s="486"/>
-      <c r="Y2" s="928" t="s">
+      <c r="Y2" s="940" t="s">
         <v>229</v>
       </c>
-      <c r="Z2" s="928"/>
-      <c r="AA2" s="928" t="s">
+      <c r="Z2" s="940"/>
+      <c r="AA2" s="940" t="s">
         <v>230</v>
       </c>
-      <c r="AB2" s="928"/>
-      <c r="AC2" s="928" t="s">
+      <c r="AB2" s="940"/>
+      <c r="AC2" s="940" t="s">
         <v>231</v>
       </c>
-      <c r="AD2" s="937"/>
-      <c r="AE2" s="932"/>
+      <c r="AD2" s="941"/>
+      <c r="AE2" s="945"/>
       <c r="AF2" s="705" t="s">
         <v>520</v>
       </c>
@@ -10104,11 +10110,6 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:AH4"/>
   <mergeCells count="18">
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="D2:E2"/>
     <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AE1:AE2"/>
     <mergeCell ref="A1:F1"/>
@@ -10122,6 +10123,11 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10311,8 +10317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U179"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10336,9 +10342,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="957"/>
-      <c r="B1" s="827"/>
-      <c r="C1" s="827"/>
+      <c r="A1" s="950"/>
+      <c r="B1" s="851"/>
+      <c r="C1" s="851"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I2" s="764"/>
@@ -10349,43 +10355,43 @@
         <v>400</v>
       </c>
       <c r="L2" s="765" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="960" t="s">
+      <c r="A3" s="958" t="s">
         <v>399</v>
       </c>
-      <c r="B3" s="962" t="s">
+      <c r="B3" s="960" t="s">
         <v>509</v>
       </c>
-      <c r="C3" s="963"/>
-      <c r="D3" s="949" t="s">
+      <c r="C3" s="961"/>
+      <c r="D3" s="956" t="s">
         <v>510</v>
       </c>
-      <c r="E3" s="950"/>
-      <c r="F3" s="949" t="s">
+      <c r="E3" s="957"/>
+      <c r="F3" s="956" t="s">
         <v>549</v>
       </c>
-      <c r="G3" s="950"/>
+      <c r="G3" s="957"/>
       <c r="I3" s="762" t="str">
         <f>$B$3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
       <c r="J3" s="763" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="K3" s="744"/>
       <c r="L3" s="744"/>
       <c r="N3" s="729"/>
-      <c r="O3" s="946" t="s">
+      <c r="O3" s="972" t="s">
         <v>400</v>
       </c>
-      <c r="P3" s="946"/>
-      <c r="Q3" s="946" t="s">
+      <c r="P3" s="972"/>
+      <c r="Q3" s="972" t="s">
         <v>401</v>
       </c>
-      <c r="R3" s="946"/>
+      <c r="R3" s="972"/>
       <c r="S3" s="729"/>
       <c r="T3" s="737" t="s">
         <v>402</v>
@@ -10393,7 +10399,7 @@
       <c r="U3" s="729"/>
     </row>
     <row r="4" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="961"/>
+      <c r="A4" s="959"/>
       <c r="B4" s="529" t="s">
         <v>403</v>
       </c>
@@ -10417,7 +10423,7 @@
         <v xml:space="preserve">[#current_year#] </v>
       </c>
       <c r="J4" s="763" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="K4" s="744"/>
       <c r="L4" s="744"/>
@@ -10465,7 +10471,7 @@
         <v xml:space="preserve">[#current_year#] </v>
       </c>
       <c r="J5" s="763" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="K5" s="744"/>
       <c r="L5" s="744"/>
@@ -10514,7 +10520,7 @@
         <v xml:space="preserve">[#current_year#] </v>
       </c>
       <c r="J6" s="763" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="K6" s="744"/>
       <c r="L6" s="744"/>
@@ -10563,7 +10569,7 @@
         <v xml:space="preserve">[#current_year#] </v>
       </c>
       <c r="J7" s="763" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="K7" s="744"/>
       <c r="L7" s="744"/>
@@ -10603,7 +10609,7 @@
         <v>[#previous_year#]</v>
       </c>
       <c r="J8" s="763" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="K8" s="744"/>
       <c r="L8" s="744"/>
@@ -10636,7 +10642,7 @@
         <v>[#previous_year#]</v>
       </c>
       <c r="J9" s="763" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="K9" s="744"/>
       <c r="L9" s="744"/>
@@ -10647,19 +10653,19 @@
         <v>[#previous_year#]</v>
       </c>
       <c r="J10" s="763" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="K10" s="744"/>
       <c r="L10" s="744"/>
       <c r="N10" s="737"/>
-      <c r="O10" s="946" t="s">
+      <c r="O10" s="972" t="s">
         <v>403</v>
       </c>
-      <c r="P10" s="946"/>
-      <c r="Q10" s="946" t="s">
+      <c r="P10" s="972"/>
+      <c r="Q10" s="972" t="s">
         <v>410</v>
       </c>
-      <c r="R10" s="946"/>
+      <c r="R10" s="972"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I11" s="762" t="str">
@@ -10667,7 +10673,7 @@
         <v>[#previous_year#]</v>
       </c>
       <c r="J11" s="763" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="K11" s="744"/>
       <c r="L11" s="744"/>
@@ -10697,7 +10703,7 @@
         <v>[#previous_year#]</v>
       </c>
       <c r="J12" s="763" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="K12" s="744"/>
       <c r="L12" s="744"/>
@@ -10723,7 +10729,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="960" t="s">
+      <c r="A13" s="958" t="s">
         <v>411</v>
       </c>
       <c r="B13" s="528" t="str">
@@ -10743,7 +10749,7 @@
         <v>[#previous_year_n2#]</v>
       </c>
       <c r="J13" s="763" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="K13" s="744"/>
       <c r="L13" s="744"/>
@@ -10769,7 +10775,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="961"/>
+      <c r="A14" s="959"/>
       <c r="B14" s="531" t="s">
         <v>404</v>
       </c>
@@ -10784,7 +10790,7 @@
         <v>[#previous_year_n2#]</v>
       </c>
       <c r="J14" s="763" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="K14" s="744"/>
       <c r="L14" s="744"/>
@@ -10821,7 +10827,7 @@
         <v>[#previous_year_n2#]</v>
       </c>
       <c r="J15" s="763" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="K15" s="744"/>
       <c r="L15" s="744"/>
@@ -10857,7 +10863,7 @@
         <v>[#previous_year_n2#]</v>
       </c>
       <c r="J16" s="763" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="K16" s="744"/>
       <c r="L16" s="744"/>
@@ -10874,7 +10880,7 @@
         <v>[#previous_year_n2#]</v>
       </c>
       <c r="J17" s="763" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="K17" s="744"/>
       <c r="L17" s="744"/>
@@ -10899,34 +10905,34 @@
       <c r="A21" s="519" t="s">
         <v>416</v>
       </c>
-      <c r="B21" s="951" t="s">
-        <v>569</v>
-      </c>
-      <c r="C21" s="952"/>
-      <c r="D21" s="952"/>
-      <c r="E21" s="952"/>
-      <c r="F21" s="952"/>
-      <c r="G21" s="952"/>
+      <c r="B21" s="974" t="s">
+        <v>568</v>
+      </c>
+      <c r="C21" s="975"/>
+      <c r="D21" s="975"/>
+      <c r="E21" s="975"/>
+      <c r="F21" s="975"/>
+      <c r="G21" s="975"/>
     </row>
     <row r="22" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="533" t="s">
         <v>380</v>
       </c>
-      <c r="B22" s="953" t="str">
+      <c r="B22" s="962" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C22" s="954"/>
-      <c r="D22" s="953" t="str">
+      <c r="C22" s="963"/>
+      <c r="D22" s="962" t="str">
         <f>D3</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E22" s="954"/>
-      <c r="F22" s="953" t="str">
+      <c r="E22" s="963"/>
+      <c r="F22" s="962" t="str">
         <f>F3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G22" s="954"/>
+      <c r="G22" s="963"/>
     </row>
     <row r="23" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="534"/>
@@ -11353,21 +11359,21 @@
       <c r="A41" s="536" t="s">
         <v>426</v>
       </c>
-      <c r="B41" s="958" t="str">
+      <c r="B41" s="952" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C41" s="959"/>
-      <c r="D41" s="947" t="str">
+      <c r="C41" s="953"/>
+      <c r="D41" s="954" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E41" s="948"/>
-      <c r="F41" s="947" t="str">
+      <c r="E41" s="955"/>
+      <c r="F41" s="954" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G41" s="948"/>
+      <c r="G41" s="955"/>
       <c r="N41" s="729"/>
       <c r="O41" s="756" t="s">
         <v>514</v>
@@ -11564,7 +11570,7 @@
     </row>
     <row r="53" spans="1:12" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="752" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B53" s="543" t="s">
         <v>428</v>
@@ -11575,12 +11581,17 @@
       <c r="D53" s="734" t="s">
         <v>439</v>
       </c>
-      <c r="E53" s="732"/>
-      <c r="F53" s="944" t="s">
+      <c r="E53" s="734" t="s">
+        <v>573</v>
+      </c>
+      <c r="F53" s="734" t="s">
+        <v>574</v>
+      </c>
+      <c r="H53" s="973" t="s">
         <v>561</v>
       </c>
-      <c r="G53" s="945"/>
-      <c r="H53" s="945"/>
+      <c r="I53" s="973"/>
+      <c r="J53" s="973"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="725" t="s">
@@ -11589,7 +11600,11 @@
       <c r="B54" s="599"/>
       <c r="C54" s="599"/>
       <c r="D54" s="735"/>
-      <c r="E54" s="732"/>
+      <c r="E54" s="735"/>
+      <c r="F54" s="735">
+        <f>D54-E54</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="725" t="s">
@@ -11598,13 +11613,14 @@
       <c r="B55" s="599"/>
       <c r="C55" s="599"/>
       <c r="D55" s="735"/>
-      <c r="E55" s="732"/>
-      <c r="F55" s="732"/>
-      <c r="G55" s="732"/>
+      <c r="E55" s="735"/>
+      <c r="F55" s="735">
+        <f t="shared" ref="F55:F62" si="8">D55-E55</f>
+        <v>0</v>
+      </c>
       <c r="H55" s="732"/>
       <c r="I55" s="732"/>
       <c r="J55" s="732"/>
-      <c r="K55" s="732"/>
       <c r="L55" s="732"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -11614,13 +11630,14 @@
       <c r="B56" s="599"/>
       <c r="C56" s="599"/>
       <c r="D56" s="735"/>
-      <c r="E56" s="732"/>
-      <c r="F56" s="732"/>
-      <c r="G56" s="732"/>
+      <c r="E56" s="735"/>
+      <c r="F56" s="735">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="H56" s="732"/>
       <c r="I56" s="732"/>
       <c r="J56" s="732"/>
-      <c r="K56" s="732"/>
       <c r="L56" s="732"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
@@ -11630,13 +11647,14 @@
       <c r="B57" s="599"/>
       <c r="C57" s="599"/>
       <c r="D57" s="735"/>
-      <c r="E57" s="732"/>
-      <c r="F57" s="732"/>
-      <c r="G57" s="732"/>
+      <c r="E57" s="735"/>
+      <c r="F57" s="735">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="H57" s="732"/>
       <c r="I57" s="732"/>
       <c r="J57" s="732"/>
-      <c r="K57" s="732"/>
       <c r="L57" s="732"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
@@ -11646,13 +11664,14 @@
       <c r="B58" s="599"/>
       <c r="C58" s="599"/>
       <c r="D58" s="735"/>
-      <c r="E58" s="732"/>
-      <c r="F58" s="732"/>
-      <c r="G58" s="732"/>
+      <c r="E58" s="735"/>
+      <c r="F58" s="735">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="H58" s="732"/>
       <c r="I58" s="732"/>
       <c r="J58" s="732"/>
-      <c r="K58" s="732"/>
       <c r="L58" s="732"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -11662,13 +11681,14 @@
       <c r="B59" s="599"/>
       <c r="C59" s="599"/>
       <c r="D59" s="735"/>
-      <c r="E59" s="732"/>
-      <c r="F59" s="732"/>
-      <c r="G59" s="732"/>
+      <c r="E59" s="735"/>
+      <c r="F59" s="735">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="H59" s="732"/>
       <c r="I59" s="732"/>
       <c r="J59" s="732"/>
-      <c r="K59" s="732"/>
       <c r="L59" s="732"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
@@ -11678,13 +11698,14 @@
       <c r="B60" s="599"/>
       <c r="C60" s="599"/>
       <c r="D60" s="735"/>
-      <c r="E60" s="732"/>
-      <c r="F60" s="732"/>
-      <c r="G60" s="732"/>
+      <c r="E60" s="735"/>
+      <c r="F60" s="735">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="H60" s="732"/>
       <c r="I60" s="732"/>
       <c r="J60" s="732"/>
-      <c r="K60" s="732"/>
       <c r="L60" s="732"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
@@ -11694,13 +11715,14 @@
       <c r="B61" s="601"/>
       <c r="C61" s="601"/>
       <c r="D61" s="735"/>
-      <c r="E61" s="732"/>
-      <c r="F61" s="732"/>
-      <c r="G61" s="732"/>
+      <c r="E61" s="735"/>
+      <c r="F61" s="735">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="H61" s="732"/>
       <c r="I61" s="732"/>
       <c r="J61" s="732"/>
-      <c r="K61" s="732"/>
       <c r="L61" s="732"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
@@ -11710,18 +11732,19 @@
       <c r="B62" s="599"/>
       <c r="C62" s="599"/>
       <c r="D62" s="735"/>
-      <c r="E62" s="732"/>
-      <c r="F62" s="732"/>
-      <c r="G62" s="732"/>
+      <c r="E62" s="735"/>
+      <c r="F62" s="735">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="H62" s="732"/>
       <c r="I62" s="732"/>
       <c r="J62" s="732"/>
-      <c r="K62" s="732"/>
       <c r="L62" s="732"/>
     </row>
     <row r="63" spans="1:12" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="753" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B63" s="544" t="s">
         <v>428</v>
@@ -11732,15 +11755,17 @@
       <c r="D63" s="734" t="s">
         <v>439</v>
       </c>
-      <c r="E63" s="732"/>
-      <c r="F63" s="944" t="s">
-        <v>562</v>
-      </c>
-      <c r="G63" s="945"/>
-      <c r="H63" s="945"/>
-      <c r="I63" s="732"/>
-      <c r="J63" s="732"/>
-      <c r="K63" s="732"/>
+      <c r="E63" s="734" t="s">
+        <v>573</v>
+      </c>
+      <c r="F63" s="734" t="s">
+        <v>574</v>
+      </c>
+      <c r="H63" s="973" t="s">
+        <v>575</v>
+      </c>
+      <c r="I63" s="973"/>
+      <c r="J63" s="973"/>
       <c r="L63" s="732"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
@@ -11750,8 +11775,11 @@
       <c r="B64" s="600"/>
       <c r="C64" s="600"/>
       <c r="D64" s="735"/>
-      <c r="E64" s="732"/>
-      <c r="F64" s="732"/>
+      <c r="E64" s="735"/>
+      <c r="F64" s="735">
+        <f>D64-E64</f>
+        <v>0</v>
+      </c>
       <c r="G64" s="732"/>
       <c r="H64" s="732"/>
       <c r="I64" s="732"/>
@@ -11766,8 +11794,11 @@
       <c r="B65" s="601"/>
       <c r="C65" s="601"/>
       <c r="D65" s="735"/>
-      <c r="E65" s="732"/>
-      <c r="F65" s="732"/>
+      <c r="E65" s="735"/>
+      <c r="F65" s="735">
+        <f t="shared" ref="F65:F72" si="9">D65-E65</f>
+        <v>0</v>
+      </c>
       <c r="G65" s="732"/>
       <c r="H65" s="732"/>
       <c r="I65" s="732"/>
@@ -11782,8 +11813,11 @@
       <c r="B66" s="601"/>
       <c r="C66" s="601"/>
       <c r="D66" s="735"/>
-      <c r="E66" s="732"/>
-      <c r="F66" s="732"/>
+      <c r="E66" s="735"/>
+      <c r="F66" s="735">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="G66" s="732"/>
       <c r="H66" s="732"/>
       <c r="I66" s="732"/>
@@ -11798,8 +11832,11 @@
       <c r="B67" s="601"/>
       <c r="C67" s="601"/>
       <c r="D67" s="735"/>
-      <c r="E67" s="732"/>
-      <c r="F67" s="732"/>
+      <c r="E67" s="735"/>
+      <c r="F67" s="735">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="G67" s="732"/>
       <c r="H67" s="732"/>
       <c r="I67" s="732"/>
@@ -11814,8 +11851,11 @@
       <c r="B68" s="601"/>
       <c r="C68" s="601"/>
       <c r="D68" s="735"/>
-      <c r="E68" s="732"/>
-      <c r="F68" s="732"/>
+      <c r="E68" s="735"/>
+      <c r="F68" s="735">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="G68" s="732"/>
       <c r="H68" s="732"/>
       <c r="I68" s="732"/>
@@ -11830,8 +11870,11 @@
       <c r="B69" s="601"/>
       <c r="C69" s="601"/>
       <c r="D69" s="735"/>
-      <c r="E69" s="732"/>
-      <c r="F69" s="732"/>
+      <c r="E69" s="735"/>
+      <c r="F69" s="735">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="G69" s="732"/>
       <c r="H69" s="732"/>
       <c r="I69" s="732"/>
@@ -11846,8 +11889,11 @@
       <c r="B70" s="601"/>
       <c r="C70" s="601"/>
       <c r="D70" s="735"/>
-      <c r="E70" s="732"/>
-      <c r="F70" s="732"/>
+      <c r="E70" s="735"/>
+      <c r="F70" s="735">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="G70" s="732"/>
       <c r="H70" s="732"/>
       <c r="I70" s="732"/>
@@ -11862,8 +11908,11 @@
       <c r="B71" s="727"/>
       <c r="C71" s="727"/>
       <c r="D71" s="736"/>
-      <c r="E71" s="732"/>
-      <c r="F71" s="732"/>
+      <c r="E71" s="736"/>
+      <c r="F71" s="735">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="G71" s="732"/>
       <c r="H71" s="732"/>
       <c r="I71" s="732"/>
@@ -11878,8 +11927,11 @@
       <c r="B72" s="729"/>
       <c r="C72" s="729"/>
       <c r="D72" s="729"/>
-      <c r="E72" s="733"/>
-      <c r="F72" s="733"/>
+      <c r="E72" s="729"/>
+      <c r="F72" s="735">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="G72" s="733"/>
       <c r="H72" s="733"/>
       <c r="I72" s="732"/>
@@ -11900,12 +11952,12 @@
       <c r="A74" s="642" t="s">
         <v>425</v>
       </c>
-      <c r="B74" s="945" t="s">
+      <c r="B74" s="951" t="s">
         <v>511</v>
       </c>
-      <c r="C74" s="945"/>
-      <c r="D74" s="945"/>
-      <c r="E74" s="945"/>
+      <c r="C74" s="951"/>
+      <c r="D74" s="951"/>
+      <c r="E74" s="951"/>
       <c r="I74" s="733"/>
       <c r="J74" s="733"/>
       <c r="K74" s="733"/>
@@ -11930,6 +11982,9 @@
       <c r="H75" s="550" t="s">
         <v>442</v>
       </c>
+      <c r="I75" s="546"/>
+      <c r="J75" s="757"/>
+      <c r="K75" s="757"/>
     </row>
     <row r="76" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="524" t="s">
@@ -11960,6 +12015,11 @@
         <f>D3</f>
         <v>[#previous_year#]</v>
       </c>
+      <c r="I76" s="641" t="s">
+        <v>290</v>
+      </c>
+      <c r="J76" s="758"/>
+      <c r="K76" s="758"/>
     </row>
     <row r="77" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="636" t="s">
@@ -11972,9 +12032,9 @@
       <c r="F77" s="577"/>
       <c r="G77" s="615"/>
       <c r="H77" s="578"/>
-      <c r="I77" s="546"/>
-      <c r="J77" s="757"/>
-      <c r="K77" s="757"/>
+      <c r="I77" s="619"/>
+      <c r="J77" s="759"/>
+      <c r="K77" s="759"/>
       <c r="N77" s="742" t="s">
         <v>443</v>
       </c>
@@ -12009,31 +12069,29 @@
       <c r="F78" s="579"/>
       <c r="G78" s="616"/>
       <c r="H78" s="580"/>
-      <c r="I78" s="641" t="s">
-        <v>290</v>
-      </c>
-      <c r="J78" s="758"/>
-      <c r="K78" s="758"/>
+      <c r="I78" s="620"/>
+      <c r="J78" s="759"/>
+      <c r="K78" s="759"/>
       <c r="N78" s="737" t="s">
         <v>444</v>
       </c>
       <c r="O78" s="744">
-        <f t="shared" ref="O78:O83" si="8">H77</f>
+        <f t="shared" ref="O78:O83" si="10">H77</f>
         <v>0</v>
       </c>
       <c r="P78" s="737">
-        <f t="shared" ref="P78:P83" si="9">D77</f>
+        <f t="shared" ref="P78:P83" si="11">D77</f>
         <v>0</v>
       </c>
       <c r="Q78" s="737" t="s">
         <v>334</v>
       </c>
       <c r="R78" s="744">
-        <f t="shared" ref="R78:R83" si="10">F77</f>
+        <f t="shared" ref="R78:R83" si="12">F77</f>
         <v>0</v>
       </c>
       <c r="S78" s="737">
-        <f t="shared" ref="S78:S83" si="11">B77</f>
+        <f t="shared" ref="S78:S83" si="13">B77</f>
         <v>0</v>
       </c>
     </row>
@@ -12048,29 +12106,29 @@
       <c r="F79" s="579"/>
       <c r="G79" s="616"/>
       <c r="H79" s="580"/>
-      <c r="I79" s="619"/>
+      <c r="I79" s="620"/>
       <c r="J79" s="759"/>
       <c r="K79" s="759"/>
       <c r="N79" s="745" t="s">
         <v>324</v>
       </c>
       <c r="O79" s="744">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P79" s="737">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q79" s="745" t="s">
         <v>324</v>
       </c>
       <c r="R79" s="744">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S79" s="737">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -12092,22 +12150,22 @@
         <v>445</v>
       </c>
       <c r="O80" s="744">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P80" s="737">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q80" s="745" t="s">
         <v>445</v>
       </c>
       <c r="R80" s="744">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S80" s="737">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -12122,29 +12180,29 @@
       <c r="F81" s="581"/>
       <c r="G81" s="617"/>
       <c r="H81" s="582"/>
-      <c r="I81" s="620"/>
-      <c r="J81" s="759"/>
-      <c r="K81" s="759"/>
+      <c r="I81" s="621"/>
+      <c r="J81" s="760"/>
+      <c r="K81" s="760"/>
       <c r="N81" s="745" t="s">
         <v>447</v>
       </c>
       <c r="O81" s="744">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P81" s="737">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q81" s="745" t="s">
         <v>446</v>
       </c>
       <c r="R81" s="744">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S81" s="737">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -12159,56 +12217,53 @@
       <c r="F82" s="583"/>
       <c r="G82" s="618"/>
       <c r="H82" s="584"/>
-      <c r="I82" s="620"/>
-      <c r="J82" s="759"/>
-      <c r="K82" s="759"/>
+      <c r="I82" s="622"/>
+      <c r="J82" s="760"/>
+      <c r="K82" s="760"/>
       <c r="N82" s="745" t="s">
         <v>448</v>
       </c>
       <c r="O82" s="744">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P82" s="737">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q82" s="745" t="s">
         <v>448</v>
       </c>
       <c r="R82" s="744">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S82" s="737">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N83" s="745" t="s">
+        <v>450</v>
+      </c>
+      <c r="O83" s="744">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="S82" s="737">
+      <c r="P83" s="737">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I83" s="621"/>
-      <c r="J83" s="760"/>
-      <c r="K83" s="760"/>
-      <c r="N83" s="745" t="s">
-        <v>450</v>
-      </c>
-      <c r="O83" s="744">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P83" s="737">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
       <c r="Q83" s="745" t="s">
         <v>449</v>
       </c>
       <c r="R83" s="744">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S83" s="737">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -12216,41 +12271,38 @@
       <c r="A84" s="553" t="s">
         <v>451</v>
       </c>
-      <c r="I84" s="622"/>
-      <c r="J84" s="760"/>
-      <c r="K84" s="760"/>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B85" s="942" t="str">
+      <c r="B85" s="966" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C85" s="943"/>
-      <c r="D85" s="942" t="str">
+      <c r="C85" s="967"/>
+      <c r="D85" s="966" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E85" s="943"/>
-      <c r="F85" s="942" t="str">
+      <c r="E85" s="967"/>
+      <c r="F85" s="966" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G85" s="943"/>
+      <c r="G85" s="967"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="520"/>
-      <c r="B86" s="899" t="s">
+      <c r="B86" s="911" t="s">
         <v>323</v>
       </c>
-      <c r="C86" s="900"/>
-      <c r="D86" s="899" t="s">
+      <c r="C86" s="912"/>
+      <c r="D86" s="911" t="s">
         <v>323</v>
       </c>
-      <c r="E86" s="900"/>
-      <c r="F86" s="899" t="s">
+      <c r="E86" s="912"/>
+      <c r="F86" s="911" t="s">
         <v>323</v>
       </c>
-      <c r="G86" s="900"/>
+      <c r="G86" s="912"/>
       <c r="N86" s="737" t="s">
         <v>452</v>
       </c>
@@ -12293,15 +12345,15 @@
         <v>453</v>
       </c>
       <c r="O87" s="737">
-        <f t="shared" ref="O87:P94" si="12">C88</f>
+        <f t="shared" ref="O87:P94" si="14">C88</f>
         <v>0</v>
       </c>
       <c r="P87" s="737">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>100</v>
       </c>
       <c r="Q87" s="737">
-        <f t="shared" ref="Q87:Q94" si="13">B88</f>
+        <f t="shared" ref="Q87:Q94" si="15">B88</f>
         <v>100</v>
       </c>
     </row>
@@ -12325,15 +12377,15 @@
         <v>454</v>
       </c>
       <c r="O88" s="737">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="P88" s="737">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q88" s="737">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -12351,15 +12403,15 @@
         <v>455</v>
       </c>
       <c r="O89" s="737">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="P89" s="737">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>100</v>
       </c>
       <c r="Q89" s="737">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>100</v>
       </c>
     </row>
@@ -12383,15 +12435,15 @@
         <v>456</v>
       </c>
       <c r="O90" s="737">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="P90" s="737">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q90" s="737">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -12409,15 +12461,15 @@
         <v>457</v>
       </c>
       <c r="O91" s="737">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="P91" s="737">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q91" s="737">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -12435,15 +12487,15 @@
         <v>458</v>
       </c>
       <c r="O92" s="737">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="P92" s="737">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>100</v>
       </c>
       <c r="Q92" s="737">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>100</v>
       </c>
     </row>
@@ -12467,15 +12519,15 @@
         <v>459</v>
       </c>
       <c r="O93" s="737">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="P93" s="737">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q93" s="737">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -12493,15 +12545,15 @@
         <v>460</v>
       </c>
       <c r="O94" s="737">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="P94" s="737">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q94" s="737">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -12531,36 +12583,36 @@
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B101" s="942" t="str">
+      <c r="B101" s="966" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C101" s="943"/>
-      <c r="D101" s="942" t="str">
+      <c r="C101" s="967"/>
+      <c r="D101" s="966" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E101" s="943"/>
-      <c r="F101" s="942" t="str">
+      <c r="E101" s="967"/>
+      <c r="F101" s="966" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G101" s="943"/>
+      <c r="G101" s="967"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="520"/>
-      <c r="B102" s="899" t="s">
+      <c r="B102" s="911" t="s">
         <v>323</v>
       </c>
-      <c r="C102" s="900"/>
-      <c r="D102" s="899" t="s">
+      <c r="C102" s="912"/>
+      <c r="D102" s="911" t="s">
         <v>323</v>
       </c>
-      <c r="E102" s="900"/>
-      <c r="F102" s="899" t="s">
+      <c r="E102" s="912"/>
+      <c r="F102" s="911" t="s">
         <v>323</v>
       </c>
-      <c r="G102" s="900"/>
+      <c r="G102" s="912"/>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" s="521" t="s">
@@ -12620,15 +12672,15 @@
         <v>453</v>
       </c>
       <c r="O104" s="731">
-        <f t="shared" ref="O104:P111" si="14">C104</f>
+        <f t="shared" ref="O104:P111" si="16">C104</f>
         <v>0</v>
       </c>
       <c r="P104" s="587">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>100</v>
       </c>
       <c r="Q104" s="587">
-        <f t="shared" ref="Q104:Q111" si="15">B104</f>
+        <f t="shared" ref="Q104:Q111" si="17">B104</f>
         <v>100</v>
       </c>
     </row>
@@ -12646,15 +12698,15 @@
         <v>454</v>
       </c>
       <c r="O105" s="731">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P105" s="587">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Q105" s="587">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12678,15 +12730,15 @@
         <v>455</v>
       </c>
       <c r="O106" s="731">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P106" s="587">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>100</v>
       </c>
       <c r="Q106" s="587">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>100</v>
       </c>
     </row>
@@ -12704,15 +12756,15 @@
         <v>456</v>
       </c>
       <c r="O107" s="731">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P107" s="587">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Q107" s="587">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12730,15 +12782,15 @@
         <v>457</v>
       </c>
       <c r="O108" s="731">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P108" s="587">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Q108" s="587">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12762,15 +12814,15 @@
         <v>458</v>
       </c>
       <c r="O109" s="731">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P109" s="587">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>100</v>
       </c>
       <c r="Q109" s="587">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>100</v>
       </c>
     </row>
@@ -12788,15 +12840,15 @@
         <v>459</v>
       </c>
       <c r="O110" s="731">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P110" s="587">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Q110" s="587">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12814,15 +12866,15 @@
         <v>460</v>
       </c>
       <c r="O111" s="731">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P111" s="587">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Q111" s="587">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12841,36 +12893,36 @@
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B116" s="938" t="str">
+      <c r="B116" s="968" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C116" s="939"/>
-      <c r="D116" s="938" t="str">
+      <c r="C116" s="969"/>
+      <c r="D116" s="968" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E116" s="939"/>
-      <c r="F116" s="938" t="str">
+      <c r="E116" s="969"/>
+      <c r="F116" s="968" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G116" s="939"/>
+      <c r="G116" s="969"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" s="559"/>
-      <c r="B117" s="940" t="s">
+      <c r="B117" s="970" t="s">
         <v>323</v>
       </c>
-      <c r="C117" s="941"/>
-      <c r="D117" s="940" t="s">
+      <c r="C117" s="971"/>
+      <c r="D117" s="970" t="s">
         <v>323</v>
       </c>
-      <c r="E117" s="941"/>
-      <c r="F117" s="940" t="s">
+      <c r="E117" s="971"/>
+      <c r="F117" s="970" t="s">
         <v>323</v>
       </c>
-      <c r="G117" s="941"/>
+      <c r="G117" s="971"/>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" s="560" t="s">
@@ -12894,6 +12946,9 @@
       <c r="G118" s="562" t="s">
         <v>105</v>
       </c>
+      <c r="I118" s="586"/>
+      <c r="J118" s="586"/>
+      <c r="K118" s="586"/>
       <c r="N118" s="737" t="s">
         <v>452</v>
       </c>
@@ -12926,19 +12981,22 @@
         <v>100</v>
       </c>
       <c r="G119" s="585"/>
+      <c r="I119" s="586"/>
+      <c r="J119" s="586"/>
+      <c r="K119" s="586"/>
       <c r="N119" s="554" t="s">
         <v>453</v>
       </c>
       <c r="O119" s="731">
-        <f t="shared" ref="O119:P126" si="16">D119</f>
+        <f t="shared" ref="O119:P126" si="18">D119</f>
         <v>100</v>
       </c>
       <c r="P119" s="587">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q119" s="588">
-        <f t="shared" ref="Q119:Q126" si="17">C119</f>
+        <f t="shared" ref="Q119:Q126" si="19">C119</f>
         <v>0</v>
       </c>
     </row>
@@ -12959,15 +13017,15 @@
         <v>454</v>
       </c>
       <c r="O120" s="731">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P120" s="587">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q120" s="588">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -12994,15 +13052,15 @@
         <v>455</v>
       </c>
       <c r="O121" s="731">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
       <c r="P121" s="587">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q121" s="588">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -13023,15 +13081,15 @@
         <v>456</v>
       </c>
       <c r="O122" s="731">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P122" s="587">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q122" s="588">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -13052,15 +13110,15 @@
         <v>457</v>
       </c>
       <c r="O123" s="646">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P123" s="576">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q123" s="588">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -13087,15 +13145,15 @@
         <v>458</v>
       </c>
       <c r="O124" s="646">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
       <c r="P124" s="576">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q124" s="588">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -13116,15 +13174,15 @@
         <v>459</v>
       </c>
       <c r="O125" s="646">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P125" s="576">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q125" s="588">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -13138,22 +13196,19 @@
       <c r="E126" s="537"/>
       <c r="F126" s="610"/>
       <c r="G126" s="601"/>
-      <c r="I126" s="586"/>
-      <c r="J126" s="586"/>
-      <c r="K126" s="586"/>
       <c r="N126" s="555" t="s">
         <v>460</v>
       </c>
       <c r="O126" s="646">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P126" s="576">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q126" s="588">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -13165,20 +13220,17 @@
       <c r="E127" s="537"/>
       <c r="F127" s="607"/>
       <c r="G127" s="601"/>
-      <c r="I127" s="586"/>
-      <c r="J127" s="586"/>
-      <c r="K127" s="586"/>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" s="563" t="s">
         <v>411</v>
       </c>
-      <c r="B129" s="955" t="str">
+      <c r="B129" s="964" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C129" s="956"/>
-      <c r="D129" s="956"/>
+      <c r="C129" s="965"/>
+      <c r="D129" s="965"/>
       <c r="N129" s="737" t="s">
         <v>452</v>
       </c>
@@ -13954,16 +14006,22 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="39">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="H63:J63"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="B129:D129"/>
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="D85:E85"/>
@@ -13977,22 +14035,16 @@
     <mergeCell ref="D116:E116"/>
     <mergeCell ref="B117:C117"/>
     <mergeCell ref="D117:E117"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F116:G116"/>
-    <mergeCell ref="F117:G117"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14835,7 +14887,7 @@
       <c r="B5" s="657" t="s">
         <v>492</v>
       </c>
-      <c r="C5" s="975" t="s">
+      <c r="C5" s="789" t="s">
         <v>495</v>
       </c>
       <c r="D5" s="657" t="s">
@@ -17381,62 +17433,62 @@
       <c r="AP3" s="7"/>
     </row>
     <row r="4" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="778" t="s">
-        <v>572</v>
-      </c>
-      <c r="B4" s="779"/>
-      <c r="C4" s="779"/>
-      <c r="D4" s="779"/>
-      <c r="E4" s="780"/>
-      <c r="F4" s="780"/>
-      <c r="G4" s="780"/>
-      <c r="H4" s="780"/>
-      <c r="I4" s="780"/>
-      <c r="J4" s="780"/>
-      <c r="K4" s="780"/>
-      <c r="L4" s="780"/>
-      <c r="M4" s="780"/>
-      <c r="N4" s="780"/>
-      <c r="O4" s="780"/>
-      <c r="P4" s="780"/>
-      <c r="Q4" s="780"/>
-      <c r="R4" s="780"/>
-      <c r="S4" s="780"/>
-      <c r="T4" s="780"/>
-      <c r="U4" s="780"/>
-      <c r="V4" s="780"/>
-      <c r="W4" s="780"/>
-      <c r="X4" s="780"/>
-      <c r="Y4" s="780"/>
-      <c r="Z4" s="780"/>
-      <c r="AA4" s="780"/>
-      <c r="AB4" s="780"/>
-      <c r="AC4" s="780"/>
-      <c r="AD4" s="780"/>
-      <c r="AE4" s="780"/>
-      <c r="AF4" s="780"/>
-      <c r="AG4" s="780"/>
-      <c r="AH4" s="780"/>
-      <c r="AI4" s="780"/>
-      <c r="AJ4" s="780"/>
-      <c r="AK4" s="780"/>
-      <c r="AL4" s="780"/>
-      <c r="AM4" s="780"/>
-      <c r="AN4" s="780"/>
-      <c r="AO4" s="780"/>
-      <c r="AP4" s="780"/>
+      <c r="A4" s="790" t="s">
+        <v>571</v>
+      </c>
+      <c r="B4" s="791"/>
+      <c r="C4" s="791"/>
+      <c r="D4" s="791"/>
+      <c r="E4" s="792"/>
+      <c r="F4" s="792"/>
+      <c r="G4" s="792"/>
+      <c r="H4" s="792"/>
+      <c r="I4" s="792"/>
+      <c r="J4" s="792"/>
+      <c r="K4" s="792"/>
+      <c r="L4" s="792"/>
+      <c r="M4" s="792"/>
+      <c r="N4" s="792"/>
+      <c r="O4" s="792"/>
+      <c r="P4" s="792"/>
+      <c r="Q4" s="792"/>
+      <c r="R4" s="792"/>
+      <c r="S4" s="792"/>
+      <c r="T4" s="792"/>
+      <c r="U4" s="792"/>
+      <c r="V4" s="792"/>
+      <c r="W4" s="792"/>
+      <c r="X4" s="792"/>
+      <c r="Y4" s="792"/>
+      <c r="Z4" s="792"/>
+      <c r="AA4" s="792"/>
+      <c r="AB4" s="792"/>
+      <c r="AC4" s="792"/>
+      <c r="AD4" s="792"/>
+      <c r="AE4" s="792"/>
+      <c r="AF4" s="792"/>
+      <c r="AG4" s="792"/>
+      <c r="AH4" s="792"/>
+      <c r="AI4" s="792"/>
+      <c r="AJ4" s="792"/>
+      <c r="AK4" s="792"/>
+      <c r="AL4" s="792"/>
+      <c r="AM4" s="792"/>
+      <c r="AN4" s="792"/>
+      <c r="AO4" s="792"/>
+      <c r="AP4" s="792"/>
     </row>
     <row r="5" spans="1:42" s="8" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="781" t="s">
+      <c r="A5" s="793" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="781" t="s">
+      <c r="B5" s="793" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="781" t="s">
+      <c r="C5" s="793" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="781" t="s">
+      <c r="D5" s="793" t="s">
         <v>63</v>
       </c>
       <c r="E5" s="14" t="s">
@@ -17496,10 +17548,10 @@
       <c r="W5" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="X5" s="783" t="s">
+      <c r="X5" s="795" t="s">
         <v>83</v>
       </c>
-      <c r="Y5" s="783" t="s">
+      <c r="Y5" s="795" t="s">
         <v>84</v>
       </c>
       <c r="Z5" s="18" t="s">
@@ -17529,7 +17581,7 @@
       <c r="AH5" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="AI5" s="783" t="s">
+      <c r="AI5" s="795" t="s">
         <v>93</v>
       </c>
       <c r="AJ5" s="18" t="s">
@@ -17538,27 +17590,27 @@
       <c r="AK5" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="AL5" s="781" t="s">
+      <c r="AL5" s="793" t="s">
         <v>96</v>
       </c>
-      <c r="AM5" s="781" t="s">
+      <c r="AM5" s="793" t="s">
         <v>97</v>
       </c>
-      <c r="AN5" s="781" t="s">
+      <c r="AN5" s="793" t="s">
         <v>98</v>
       </c>
-      <c r="AO5" s="781" t="s">
+      <c r="AO5" s="793" t="s">
         <v>99</v>
       </c>
-      <c r="AP5" s="781" t="s">
+      <c r="AP5" s="793" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:42" s="11" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="782"/>
-      <c r="B6" s="782"/>
-      <c r="C6" s="782"/>
-      <c r="D6" s="782"/>
+      <c r="A6" s="794"/>
+      <c r="B6" s="794"/>
+      <c r="C6" s="794"/>
+      <c r="D6" s="794"/>
       <c r="E6" s="16" t="s">
         <v>101</v>
       </c>
@@ -17616,8 +17668,8 @@
       <c r="W6" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="X6" s="784"/>
-      <c r="Y6" s="784"/>
+      <c r="X6" s="796"/>
+      <c r="Y6" s="796"/>
       <c r="Z6" s="11" t="s">
         <v>102</v>
       </c>
@@ -17645,18 +17697,18 @@
       <c r="AH6" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="AI6" s="784"/>
+      <c r="AI6" s="796"/>
       <c r="AJ6" s="11" t="s">
         <v>102</v>
       </c>
       <c r="AK6" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="AL6" s="782"/>
-      <c r="AM6" s="782"/>
-      <c r="AN6" s="782"/>
-      <c r="AO6" s="782"/>
-      <c r="AP6" s="782"/>
+      <c r="AL6" s="794"/>
+      <c r="AM6" s="794"/>
+      <c r="AN6" s="794"/>
+      <c r="AO6" s="794"/>
+      <c r="AP6" s="794"/>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.3">
       <c r="AD7" s="10"/>
@@ -57711,7 +57763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
@@ -57739,8 +57791,8 @@
       <c r="B5" s="671" t="s">
         <v>498</v>
       </c>
-      <c r="C5" s="975" t="s">
-        <v>573</v>
+      <c r="C5" s="789" t="s">
+        <v>572</v>
       </c>
       <c r="D5" s="671" t="s">
         <v>499</v>
@@ -57748,7 +57800,7 @@
       <c r="E5" s="671" t="s">
         <v>500</v>
       </c>
-      <c r="F5" s="975" t="s">
+      <c r="F5" s="789" t="s">
         <v>495</v>
       </c>
       <c r="G5" s="671" t="s">
@@ -57792,98 +57844,98 @@
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="40.21875" style="965" customWidth="1"/>
+    <col min="3" max="3" width="40.21875" style="779" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="40.21875" style="965" customWidth="1"/>
+    <col min="6" max="6" width="40.21875" style="779" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="27.33203125" customWidth="1"/>
-    <col min="9" max="9" width="40.21875" style="965" customWidth="1"/>
+    <col min="9" max="9" width="40.21875" style="779" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="27.33203125" customWidth="1"/>
-    <col min="12" max="12" width="40.21875" style="965" customWidth="1"/>
+    <col min="12" max="12" width="40.21875" style="779" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
     <col min="14" max="14" width="27.33203125" customWidth="1"/>
-    <col min="15" max="15" width="40.21875" style="965" customWidth="1"/>
+    <col min="15" max="15" width="40.21875" style="779" customWidth="1"/>
     <col min="16" max="16" width="17" customWidth="1"/>
     <col min="17" max="17" width="27.33203125" customWidth="1"/>
-    <col min="18" max="18" width="40.21875" style="965" customWidth="1"/>
+    <col min="18" max="18" width="40.21875" style="779" customWidth="1"/>
     <col min="19" max="19" width="17" customWidth="1"/>
     <col min="20" max="20" width="27.33203125" customWidth="1"/>
-    <col min="21" max="21" width="40.21875" style="965" customWidth="1"/>
+    <col min="21" max="21" width="40.21875" style="779" customWidth="1"/>
     <col min="22" max="22" width="17" customWidth="1"/>
     <col min="23" max="23" width="27.33203125" customWidth="1"/>
-    <col min="24" max="24" width="40.21875" style="965" customWidth="1"/>
+    <col min="24" max="24" width="40.21875" style="779" customWidth="1"/>
     <col min="25" max="25" width="17" customWidth="1"/>
     <col min="26" max="26" width="27.33203125" customWidth="1"/>
-    <col min="27" max="27" width="40.21875" style="965" customWidth="1"/>
+    <col min="27" max="27" width="40.21875" style="779" customWidth="1"/>
     <col min="28" max="28" width="17" customWidth="1"/>
-    <col min="30" max="30" width="40.21875" style="965" customWidth="1"/>
+    <col min="30" max="30" width="40.21875" style="779" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="777" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="793"/>
-      <c r="B1" s="793"/>
-      <c r="C1" s="793"/>
-      <c r="D1" s="794"/>
-      <c r="E1" s="795"/>
-      <c r="F1" s="795"/>
-      <c r="G1" s="796"/>
-      <c r="H1" s="797"/>
-      <c r="I1" s="797"/>
-      <c r="J1" s="798"/>
-      <c r="K1" s="799"/>
-      <c r="L1" s="799"/>
-      <c r="M1" s="800"/>
-      <c r="N1" s="801"/>
-      <c r="O1" s="801"/>
-      <c r="P1" s="802"/>
-      <c r="Q1" s="803"/>
-      <c r="R1" s="803"/>
-      <c r="S1" s="785"/>
-      <c r="T1" s="786"/>
-      <c r="U1" s="786"/>
-      <c r="V1" s="787"/>
-      <c r="W1" s="788"/>
-      <c r="X1" s="788"/>
-      <c r="Y1" s="789"/>
-      <c r="Z1" s="790"/>
-      <c r="AA1" s="790"/>
-      <c r="AB1" s="791"/>
-      <c r="AC1" s="792"/>
-      <c r="AD1" s="792"/>
+      <c r="A1" s="805"/>
+      <c r="B1" s="805"/>
+      <c r="C1" s="805"/>
+      <c r="D1" s="806"/>
+      <c r="E1" s="807"/>
+      <c r="F1" s="807"/>
+      <c r="G1" s="808"/>
+      <c r="H1" s="809"/>
+      <c r="I1" s="809"/>
+      <c r="J1" s="810"/>
+      <c r="K1" s="811"/>
+      <c r="L1" s="811"/>
+      <c r="M1" s="812"/>
+      <c r="N1" s="813"/>
+      <c r="O1" s="813"/>
+      <c r="P1" s="814"/>
+      <c r="Q1" s="815"/>
+      <c r="R1" s="815"/>
+      <c r="S1" s="797"/>
+      <c r="T1" s="798"/>
+      <c r="U1" s="798"/>
+      <c r="V1" s="799"/>
+      <c r="W1" s="800"/>
+      <c r="X1" s="800"/>
+      <c r="Y1" s="801"/>
+      <c r="Z1" s="802"/>
+      <c r="AA1" s="802"/>
+      <c r="AB1" s="803"/>
+      <c r="AC1" s="804"/>
+      <c r="AD1" s="804"/>
     </row>
     <row r="2" spans="1:30" s="776" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="766"/>
       <c r="B2" s="766"/>
-      <c r="C2" s="966"/>
+      <c r="C2" s="780"/>
       <c r="D2" s="767"/>
       <c r="E2" s="767"/>
-      <c r="F2" s="964"/>
+      <c r="F2" s="778"/>
       <c r="G2" s="768"/>
       <c r="H2" s="768"/>
-      <c r="I2" s="967"/>
+      <c r="I2" s="781"/>
       <c r="J2" s="769"/>
       <c r="K2" s="769"/>
-      <c r="L2" s="968"/>
+      <c r="L2" s="782"/>
       <c r="M2" s="770"/>
       <c r="N2" s="770"/>
-      <c r="O2" s="969"/>
+      <c r="O2" s="783"/>
       <c r="P2" s="771"/>
       <c r="Q2" s="771"/>
-      <c r="R2" s="970"/>
+      <c r="R2" s="784"/>
       <c r="S2" s="772"/>
       <c r="T2" s="772"/>
-      <c r="U2" s="971"/>
+      <c r="U2" s="785"/>
       <c r="V2" s="773"/>
       <c r="W2" s="773"/>
-      <c r="X2" s="972"/>
+      <c r="X2" s="786"/>
       <c r="Y2" s="774"/>
       <c r="Z2" s="774"/>
-      <c r="AA2" s="973"/>
+      <c r="AA2" s="787"/>
       <c r="AB2" s="775"/>
       <c r="AC2" s="775"/>
-      <c r="AD2" s="974"/>
+      <c r="AD2" s="788"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -57924,10 +57976,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="804" t="s">
+      <c r="A1" s="816" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="806" t="s">
+      <c r="B1" s="818" t="s">
         <v>61</v>
       </c>
       <c r="C1" s="687" t="s">
@@ -57977,8 +58029,8 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="805"/>
-      <c r="B2" s="807"/>
+      <c r="A2" s="817"/>
+      <c r="B2" s="819"/>
       <c r="C2" s="11" t="s">
         <v>102</v>
       </c>
@@ -58141,123 +58193,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:95" s="678" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="837" t="s">
+      <c r="A1" s="820" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="838"/>
-      <c r="C1" s="838"/>
-      <c r="D1" s="838"/>
-      <c r="E1" s="838"/>
-      <c r="F1" s="838"/>
-      <c r="G1" s="838"/>
-      <c r="H1" s="839" t="s">
+      <c r="B1" s="821"/>
+      <c r="C1" s="821"/>
+      <c r="D1" s="821"/>
+      <c r="E1" s="821"/>
+      <c r="F1" s="821"/>
+      <c r="G1" s="821"/>
+      <c r="H1" s="822" t="s">
         <v>520</v>
       </c>
-      <c r="I1" s="840"/>
-      <c r="J1" s="840"/>
-      <c r="K1" s="840"/>
-      <c r="L1" s="840"/>
-      <c r="M1" s="841"/>
-      <c r="N1" s="842" t="s">
+      <c r="I1" s="823"/>
+      <c r="J1" s="823"/>
+      <c r="K1" s="823"/>
+      <c r="L1" s="823"/>
+      <c r="M1" s="824"/>
+      <c r="N1" s="825" t="s">
         <v>117</v>
       </c>
-      <c r="O1" s="820"/>
-      <c r="P1" s="820"/>
-      <c r="Q1" s="820"/>
-      <c r="R1" s="820"/>
-      <c r="S1" s="820"/>
-      <c r="T1" s="820"/>
-      <c r="U1" s="820"/>
-      <c r="V1" s="843" t="s">
+      <c r="O1" s="826"/>
+      <c r="P1" s="826"/>
+      <c r="Q1" s="826"/>
+      <c r="R1" s="826"/>
+      <c r="S1" s="826"/>
+      <c r="T1" s="826"/>
+      <c r="U1" s="826"/>
+      <c r="V1" s="827" t="s">
         <v>118</v>
       </c>
-      <c r="W1" s="844"/>
-      <c r="X1" s="845"/>
-      <c r="Y1" s="845"/>
-      <c r="Z1" s="846"/>
-      <c r="AA1" s="847" t="s">
+      <c r="W1" s="828"/>
+      <c r="X1" s="829"/>
+      <c r="Y1" s="829"/>
+      <c r="Z1" s="830"/>
+      <c r="AA1" s="831" t="s">
         <v>119</v>
       </c>
-      <c r="AB1" s="848"/>
-      <c r="AC1" s="848"/>
-      <c r="AD1" s="848"/>
-      <c r="AE1" s="848"/>
-      <c r="AF1" s="848"/>
-      <c r="AG1" s="848"/>
-      <c r="AH1" s="848"/>
-      <c r="AI1" s="848"/>
-      <c r="AJ1" s="848"/>
-      <c r="AK1" s="848"/>
-      <c r="AL1" s="848"/>
-      <c r="AM1" s="848"/>
+      <c r="AB1" s="832"/>
+      <c r="AC1" s="832"/>
+      <c r="AD1" s="832"/>
+      <c r="AE1" s="832"/>
+      <c r="AF1" s="832"/>
+      <c r="AG1" s="832"/>
+      <c r="AH1" s="832"/>
+      <c r="AI1" s="832"/>
+      <c r="AJ1" s="832"/>
+      <c r="AK1" s="832"/>
+      <c r="AL1" s="832"/>
+      <c r="AM1" s="832"/>
       <c r="AN1" s="54"/>
       <c r="AO1" s="55"/>
-      <c r="AP1" s="819" t="s">
+      <c r="AP1" s="844" t="s">
         <v>120</v>
       </c>
-      <c r="AQ1" s="820"/>
-      <c r="AR1" s="820"/>
-      <c r="AS1" s="820"/>
-      <c r="AT1" s="820"/>
-      <c r="AU1" s="820"/>
-      <c r="AV1" s="820"/>
-      <c r="AW1" s="821"/>
-      <c r="AX1" s="828" t="s">
+      <c r="AQ1" s="826"/>
+      <c r="AR1" s="826"/>
+      <c r="AS1" s="826"/>
+      <c r="AT1" s="826"/>
+      <c r="AU1" s="826"/>
+      <c r="AV1" s="826"/>
+      <c r="AW1" s="845"/>
+      <c r="AX1" s="852" t="s">
         <v>121</v>
       </c>
-      <c r="AY1" s="829"/>
-      <c r="AZ1" s="829"/>
-      <c r="BA1" s="829"/>
-      <c r="BB1" s="829"/>
-      <c r="BC1" s="830"/>
-      <c r="BD1" s="831" t="s">
+      <c r="AY1" s="853"/>
+      <c r="AZ1" s="853"/>
+      <c r="BA1" s="853"/>
+      <c r="BB1" s="853"/>
+      <c r="BC1" s="854"/>
+      <c r="BD1" s="855" t="s">
         <v>122</v>
       </c>
-      <c r="BE1" s="832"/>
-      <c r="BF1" s="832"/>
-      <c r="BG1" s="832"/>
-      <c r="BH1" s="832"/>
-      <c r="BI1" s="833"/>
-      <c r="BJ1" s="834" t="s">
+      <c r="BE1" s="856"/>
+      <c r="BF1" s="856"/>
+      <c r="BG1" s="856"/>
+      <c r="BH1" s="856"/>
+      <c r="BI1" s="857"/>
+      <c r="BJ1" s="858" t="s">
         <v>123</v>
       </c>
-      <c r="BK1" s="835"/>
-      <c r="BL1" s="835"/>
-      <c r="BM1" s="835"/>
-      <c r="BN1" s="835"/>
-      <c r="BO1" s="835"/>
-      <c r="BP1" s="836"/>
-      <c r="BQ1" s="808" t="s">
+      <c r="BK1" s="859"/>
+      <c r="BL1" s="859"/>
+      <c r="BM1" s="859"/>
+      <c r="BN1" s="859"/>
+      <c r="BO1" s="859"/>
+      <c r="BP1" s="860"/>
+      <c r="BQ1" s="833" t="s">
         <v>124</v>
       </c>
-      <c r="BR1" s="809"/>
-      <c r="BS1" s="809"/>
-      <c r="BT1" s="809"/>
-      <c r="BU1" s="809"/>
-      <c r="BV1" s="809"/>
+      <c r="BR1" s="834"/>
+      <c r="BS1" s="834"/>
+      <c r="BT1" s="834"/>
+      <c r="BU1" s="834"/>
+      <c r="BV1" s="834"/>
       <c r="BW1" s="55"/>
       <c r="BX1" s="56"/>
-      <c r="BY1" s="810" t="s">
+      <c r="BY1" s="835" t="s">
         <v>125</v>
       </c>
-      <c r="BZ1" s="811"/>
-      <c r="CA1" s="811"/>
-      <c r="CB1" s="811"/>
-      <c r="CC1" s="811"/>
-      <c r="CD1" s="811"/>
-      <c r="CE1" s="811"/>
-      <c r="CF1" s="812"/>
-      <c r="CG1" s="812"/>
-      <c r="CH1" s="812"/>
-      <c r="CI1" s="812"/>
-      <c r="CJ1" s="812"/>
-      <c r="CK1" s="812"/>
-      <c r="CL1" s="812"/>
-      <c r="CM1" s="812"/>
-      <c r="CN1" s="812"/>
-      <c r="CO1" s="812"/>
-      <c r="CP1" s="812"/>
-      <c r="CQ1" s="812"/>
+      <c r="BZ1" s="836"/>
+      <c r="CA1" s="836"/>
+      <c r="CB1" s="836"/>
+      <c r="CC1" s="836"/>
+      <c r="CD1" s="836"/>
+      <c r="CE1" s="836"/>
+      <c r="CF1" s="837"/>
+      <c r="CG1" s="837"/>
+      <c r="CH1" s="837"/>
+      <c r="CI1" s="837"/>
+      <c r="CJ1" s="837"/>
+      <c r="CK1" s="837"/>
+      <c r="CL1" s="837"/>
+      <c r="CM1" s="837"/>
+      <c r="CN1" s="837"/>
+      <c r="CO1" s="837"/>
+      <c r="CP1" s="837"/>
+      <c r="CQ1" s="837"/>
     </row>
     <row r="2" spans="1:95" s="678" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="57" t="s">
@@ -58281,18 +58333,18 @@
       <c r="G2" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="H2" s="813" t="s">
+      <c r="H2" s="838" t="s">
         <v>521</v>
       </c>
-      <c r="I2" s="814"/>
-      <c r="J2" s="814" t="s">
+      <c r="I2" s="839"/>
+      <c r="J2" s="839" t="s">
         <v>133</v>
       </c>
-      <c r="K2" s="814"/>
-      <c r="L2" s="814" t="s">
+      <c r="K2" s="839"/>
+      <c r="L2" s="839" t="s">
         <v>134</v>
       </c>
-      <c r="M2" s="815"/>
+      <c r="M2" s="840"/>
       <c r="N2" s="59" t="s">
         <v>126</v>
       </c>
@@ -58401,36 +58453,36 @@
       <c r="AW2" s="61" t="s">
         <v>164</v>
       </c>
-      <c r="AX2" s="816" t="s">
+      <c r="AX2" s="841" t="s">
         <v>165</v>
       </c>
-      <c r="AY2" s="817"/>
-      <c r="AZ2" s="817"/>
-      <c r="BA2" s="817" t="s">
+      <c r="AY2" s="842"/>
+      <c r="AZ2" s="842"/>
+      <c r="BA2" s="842" t="s">
         <v>166</v>
       </c>
-      <c r="BB2" s="817"/>
-      <c r="BC2" s="818"/>
-      <c r="BD2" s="822" t="s">
+      <c r="BB2" s="842"/>
+      <c r="BC2" s="843"/>
+      <c r="BD2" s="846" t="s">
         <v>165</v>
       </c>
-      <c r="BE2" s="823"/>
-      <c r="BF2" s="823"/>
-      <c r="BG2" s="823" t="s">
+      <c r="BE2" s="847"/>
+      <c r="BF2" s="847"/>
+      <c r="BG2" s="847" t="s">
         <v>166</v>
       </c>
-      <c r="BH2" s="823"/>
-      <c r="BI2" s="824"/>
-      <c r="BJ2" s="825" t="s">
+      <c r="BH2" s="847"/>
+      <c r="BI2" s="848"/>
+      <c r="BJ2" s="849" t="s">
         <v>165</v>
       </c>
-      <c r="BK2" s="826"/>
-      <c r="BL2" s="826"/>
-      <c r="BM2" s="826" t="s">
+      <c r="BK2" s="850"/>
+      <c r="BL2" s="850"/>
+      <c r="BM2" s="850" t="s">
         <v>166</v>
       </c>
-      <c r="BN2" s="827"/>
-      <c r="BO2" s="827"/>
+      <c r="BN2" s="851"/>
+      <c r="BO2" s="851"/>
       <c r="BP2" s="71" t="s">
         <v>167</v>
       </c>
@@ -59063,11 +59115,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AM1"/>
     <mergeCell ref="BQ1:BV1"/>
     <mergeCell ref="BY1:CQ1"/>
     <mergeCell ref="H2:I2"/>
@@ -59083,6 +59130,11 @@
     <mergeCell ref="AX1:BC1"/>
     <mergeCell ref="BD1:BI1"/>
     <mergeCell ref="BJ1:BP1"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -59165,127 +59217,127 @@
         <v>207</v>
       </c>
       <c r="L1" s="147"/>
-      <c r="M1" s="872" t="s">
+      <c r="M1" s="861" t="s">
         <v>208</v>
       </c>
-      <c r="N1" s="873" t="s">
+      <c r="N1" s="862" t="s">
         <v>209</v>
       </c>
-      <c r="O1" s="874"/>
-      <c r="P1" s="874"/>
-      <c r="Q1" s="874"/>
-      <c r="R1" s="875" t="s">
+      <c r="O1" s="863"/>
+      <c r="P1" s="863"/>
+      <c r="Q1" s="863"/>
+      <c r="R1" s="864" t="s">
         <v>520</v>
       </c>
-      <c r="S1" s="868"/>
-      <c r="T1" s="868"/>
-      <c r="U1" s="868"/>
-      <c r="V1" s="868"/>
-      <c r="W1" s="868"/>
-      <c r="X1" s="876"/>
-      <c r="Y1" s="862" t="s">
+      <c r="S1" s="865"/>
+      <c r="T1" s="865"/>
+      <c r="U1" s="865"/>
+      <c r="V1" s="865"/>
+      <c r="W1" s="865"/>
+      <c r="X1" s="866"/>
+      <c r="Y1" s="867" t="s">
         <v>528</v>
       </c>
-      <c r="Z1" s="832"/>
-      <c r="AA1" s="877" t="s">
+      <c r="Z1" s="856"/>
+      <c r="AA1" s="870" t="s">
         <v>210</v>
       </c>
-      <c r="AB1" s="850" t="s">
+      <c r="AB1" s="881" t="s">
         <v>211</v>
       </c>
-      <c r="AC1" s="864" t="s">
+      <c r="AC1" s="877" t="s">
         <v>212</v>
       </c>
-      <c r="AD1" s="865"/>
-      <c r="AE1" s="865"/>
-      <c r="AF1" s="866"/>
-      <c r="AG1" s="867" t="s">
+      <c r="AD1" s="878"/>
+      <c r="AE1" s="878"/>
+      <c r="AF1" s="879"/>
+      <c r="AG1" s="880" t="s">
         <v>213</v>
       </c>
-      <c r="AH1" s="868"/>
-      <c r="AI1" s="868"/>
-      <c r="AJ1" s="868"/>
-      <c r="AK1" s="868"/>
-      <c r="AL1" s="868"/>
-      <c r="AM1" s="868"/>
-      <c r="AN1" s="868"/>
-      <c r="AO1" s="850" t="s">
+      <c r="AH1" s="865"/>
+      <c r="AI1" s="865"/>
+      <c r="AJ1" s="865"/>
+      <c r="AK1" s="865"/>
+      <c r="AL1" s="865"/>
+      <c r="AM1" s="865"/>
+      <c r="AN1" s="865"/>
+      <c r="AO1" s="881" t="s">
         <v>214</v>
       </c>
-      <c r="AP1" s="862" t="s">
+      <c r="AP1" s="867" t="s">
         <v>527</v>
       </c>
-      <c r="AQ1" s="832"/>
-      <c r="AR1" s="832"/>
-      <c r="AS1" s="833"/>
-      <c r="AT1" s="870" t="s">
+      <c r="AQ1" s="856"/>
+      <c r="AR1" s="856"/>
+      <c r="AS1" s="857"/>
+      <c r="AT1" s="884" t="s">
         <v>215</v>
       </c>
-      <c r="AU1" s="871"/>
-      <c r="AV1" s="871"/>
-      <c r="AW1" s="871"/>
-      <c r="AX1" s="871"/>
-      <c r="AY1" s="871"/>
-      <c r="AZ1" s="871"/>
-      <c r="BA1" s="871"/>
-      <c r="BB1" s="871"/>
-      <c r="BC1" s="871"/>
-      <c r="BD1" s="871"/>
-      <c r="BE1" s="871"/>
-      <c r="BF1" s="871"/>
-      <c r="BG1" s="871"/>
-      <c r="BH1" s="871"/>
-      <c r="BI1" s="871"/>
-      <c r="BJ1" s="871"/>
-      <c r="BK1" s="871"/>
-      <c r="BL1" s="871"/>
-      <c r="BM1" s="871"/>
-      <c r="BN1" s="871"/>
-      <c r="BO1" s="871"/>
-      <c r="BP1" s="871"/>
-      <c r="BQ1" s="871"/>
-      <c r="BR1" s="871"/>
-      <c r="BS1" s="871"/>
-      <c r="BT1" s="871"/>
-      <c r="BU1" s="871"/>
-      <c r="BV1" s="871"/>
-      <c r="BW1" s="850" t="s">
+      <c r="AU1" s="885"/>
+      <c r="AV1" s="885"/>
+      <c r="AW1" s="885"/>
+      <c r="AX1" s="885"/>
+      <c r="AY1" s="885"/>
+      <c r="AZ1" s="885"/>
+      <c r="BA1" s="885"/>
+      <c r="BB1" s="885"/>
+      <c r="BC1" s="885"/>
+      <c r="BD1" s="885"/>
+      <c r="BE1" s="885"/>
+      <c r="BF1" s="885"/>
+      <c r="BG1" s="885"/>
+      <c r="BH1" s="885"/>
+      <c r="BI1" s="885"/>
+      <c r="BJ1" s="885"/>
+      <c r="BK1" s="885"/>
+      <c r="BL1" s="885"/>
+      <c r="BM1" s="885"/>
+      <c r="BN1" s="885"/>
+      <c r="BO1" s="885"/>
+      <c r="BP1" s="885"/>
+      <c r="BQ1" s="885"/>
+      <c r="BR1" s="885"/>
+      <c r="BS1" s="885"/>
+      <c r="BT1" s="885"/>
+      <c r="BU1" s="885"/>
+      <c r="BV1" s="885"/>
+      <c r="BW1" s="881" t="s">
         <v>216</v>
       </c>
-      <c r="BX1" s="862" t="s">
+      <c r="BX1" s="867" t="s">
         <v>526</v>
       </c>
-      <c r="BY1" s="832"/>
-      <c r="BZ1" s="832"/>
-      <c r="CA1" s="833"/>
-      <c r="CB1" s="861" t="s">
+      <c r="BY1" s="856"/>
+      <c r="BZ1" s="856"/>
+      <c r="CA1" s="857"/>
+      <c r="CB1" s="893" t="s">
         <v>548</v>
       </c>
-      <c r="CC1" s="863" t="s">
+      <c r="CC1" s="875" t="s">
         <v>119</v>
       </c>
-      <c r="CD1" s="863"/>
-      <c r="CE1" s="863"/>
-      <c r="CF1" s="863"/>
-      <c r="CG1" s="863"/>
-      <c r="CH1" s="863"/>
-      <c r="CI1" s="863"/>
-      <c r="CJ1" s="863"/>
-      <c r="CK1" s="863"/>
-      <c r="CL1" s="863"/>
-      <c r="CM1" s="863"/>
-      <c r="CN1" s="863"/>
+      <c r="CD1" s="875"/>
+      <c r="CE1" s="875"/>
+      <c r="CF1" s="875"/>
+      <c r="CG1" s="875"/>
+      <c r="CH1" s="875"/>
+      <c r="CI1" s="875"/>
+      <c r="CJ1" s="875"/>
+      <c r="CK1" s="875"/>
+      <c r="CL1" s="875"/>
+      <c r="CM1" s="875"/>
+      <c r="CN1" s="875"/>
       <c r="CO1" s="148"/>
-      <c r="CP1" s="849" t="s">
+      <c r="CP1" s="889" t="s">
         <v>124</v>
       </c>
-      <c r="CQ1" s="820"/>
-      <c r="CR1" s="820"/>
-      <c r="CS1" s="820"/>
-      <c r="CT1" s="820"/>
-      <c r="CU1" s="820"/>
-      <c r="CV1" s="820"/>
-      <c r="CW1" s="821"/>
+      <c r="CQ1" s="826"/>
+      <c r="CR1" s="826"/>
+      <c r="CS1" s="826"/>
+      <c r="CT1" s="826"/>
+      <c r="CU1" s="826"/>
+      <c r="CV1" s="826"/>
+      <c r="CW1" s="845"/>
     </row>
     <row r="2" spans="1:104" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="149" t="s">
@@ -59324,7 +59376,7 @@
       <c r="L2" s="153" t="s">
         <v>127</v>
       </c>
-      <c r="M2" s="872"/>
+      <c r="M2" s="861"/>
       <c r="N2" s="154" t="s">
         <v>221</v>
       </c>
@@ -59340,22 +59392,22 @@
       <c r="R2" s="159" t="s">
         <v>224</v>
       </c>
-      <c r="S2" s="879" t="s">
+      <c r="S2" s="872" t="s">
         <v>521</v>
       </c>
-      <c r="T2" s="827"/>
-      <c r="U2" s="880" t="s">
+      <c r="T2" s="851"/>
+      <c r="U2" s="873" t="s">
         <v>133</v>
       </c>
-      <c r="V2" s="880"/>
-      <c r="W2" s="880" t="s">
+      <c r="V2" s="873"/>
+      <c r="W2" s="873" t="s">
         <v>134</v>
       </c>
-      <c r="X2" s="881"/>
-      <c r="Y2" s="856"/>
-      <c r="Z2" s="857"/>
-      <c r="AA2" s="878"/>
-      <c r="AB2" s="851"/>
+      <c r="X2" s="874"/>
+      <c r="Y2" s="868"/>
+      <c r="Z2" s="869"/>
+      <c r="AA2" s="871"/>
+      <c r="AB2" s="882"/>
       <c r="AC2" s="155" t="s">
         <v>225</v>
       </c>
@@ -59368,81 +59420,81 @@
       <c r="AF2" s="155" t="s">
         <v>228</v>
       </c>
-      <c r="AG2" s="869" t="s">
+      <c r="AG2" s="883" t="s">
         <v>229</v>
       </c>
-      <c r="AH2" s="854"/>
-      <c r="AI2" s="854" t="s">
+      <c r="AH2" s="876"/>
+      <c r="AI2" s="876" t="s">
         <v>230</v>
       </c>
-      <c r="AJ2" s="854"/>
-      <c r="AK2" s="854" t="s">
+      <c r="AJ2" s="876"/>
+      <c r="AK2" s="876" t="s">
         <v>231</v>
       </c>
-      <c r="AL2" s="854"/>
+      <c r="AL2" s="876"/>
       <c r="AM2" s="156" t="s">
         <v>232</v>
       </c>
       <c r="AN2" s="156" t="s">
         <v>233</v>
       </c>
-      <c r="AO2" s="851"/>
-      <c r="AP2" s="856" t="s">
+      <c r="AO2" s="882"/>
+      <c r="AP2" s="868" t="s">
         <v>234</v>
       </c>
-      <c r="AQ2" s="857"/>
-      <c r="AR2" s="858" t="s">
+      <c r="AQ2" s="869"/>
+      <c r="AR2" s="886" t="s">
         <v>235</v>
       </c>
-      <c r="AS2" s="859"/>
-      <c r="AT2" s="854" t="s">
+      <c r="AS2" s="887"/>
+      <c r="AT2" s="876" t="s">
         <v>236</v>
       </c>
-      <c r="AU2" s="854"/>
-      <c r="AV2" s="855" t="s">
+      <c r="AU2" s="876"/>
+      <c r="AV2" s="888" t="s">
         <v>237</v>
       </c>
-      <c r="AW2" s="855"/>
-      <c r="AX2" s="855" t="s">
+      <c r="AW2" s="888"/>
+      <c r="AX2" s="888" t="s">
         <v>238</v>
       </c>
-      <c r="AY2" s="855"/>
+      <c r="AY2" s="888"/>
       <c r="AZ2" s="156" t="s">
         <v>239</v>
       </c>
       <c r="BA2" s="156" t="s">
         <v>240</v>
       </c>
-      <c r="BB2" s="854" t="s">
+      <c r="BB2" s="876" t="s">
         <v>241</v>
       </c>
-      <c r="BC2" s="854"/>
-      <c r="BD2" s="855" t="s">
+      <c r="BC2" s="876"/>
+      <c r="BD2" s="888" t="s">
         <v>242</v>
       </c>
-      <c r="BE2" s="855"/>
-      <c r="BF2" s="855" t="s">
+      <c r="BE2" s="888"/>
+      <c r="BF2" s="888" t="s">
         <v>243</v>
       </c>
-      <c r="BG2" s="855"/>
+      <c r="BG2" s="888"/>
       <c r="BH2" s="156" t="s">
         <v>244</v>
       </c>
       <c r="BI2" s="156" t="s">
         <v>245</v>
       </c>
-      <c r="BJ2" s="854" t="s">
+      <c r="BJ2" s="876" t="s">
         <v>246</v>
       </c>
-      <c r="BK2" s="854"/>
-      <c r="BL2" s="855" t="s">
+      <c r="BK2" s="876"/>
+      <c r="BL2" s="888" t="s">
         <v>247</v>
       </c>
-      <c r="BM2" s="855"/>
-      <c r="BN2" s="855" t="s">
+      <c r="BM2" s="888"/>
+      <c r="BN2" s="888" t="s">
         <v>248</v>
       </c>
-      <c r="BO2" s="855"/>
+      <c r="BO2" s="888"/>
       <c r="BP2" s="156" t="s">
         <v>249</v>
       </c>
@@ -59464,16 +59516,16 @@
       <c r="BV2" s="156" t="s">
         <v>255</v>
       </c>
-      <c r="BW2" s="851"/>
-      <c r="BX2" s="856" t="s">
+      <c r="BW2" s="882"/>
+      <c r="BX2" s="868" t="s">
         <v>234</v>
       </c>
-      <c r="BY2" s="857"/>
-      <c r="BZ2" s="858" t="s">
+      <c r="BY2" s="869"/>
+      <c r="BZ2" s="886" t="s">
         <v>235</v>
       </c>
-      <c r="CA2" s="859"/>
-      <c r="CB2" s="861"/>
+      <c r="CA2" s="887"/>
+      <c r="CB2" s="893"/>
       <c r="CC2" s="140" t="s">
         <v>144</v>
       </c>
@@ -59513,22 +59565,22 @@
       <c r="CO2" s="142" t="s">
         <v>530</v>
       </c>
-      <c r="CP2" s="860" t="s">
+      <c r="CP2" s="892" t="s">
         <v>257</v>
       </c>
-      <c r="CQ2" s="852"/>
-      <c r="CR2" s="852" t="s">
+      <c r="CQ2" s="890"/>
+      <c r="CR2" s="890" t="s">
         <v>258</v>
       </c>
-      <c r="CS2" s="852"/>
-      <c r="CT2" s="852" t="s">
+      <c r="CS2" s="890"/>
+      <c r="CT2" s="890" t="s">
         <v>259</v>
       </c>
-      <c r="CU2" s="852"/>
-      <c r="CV2" s="852" t="s">
+      <c r="CU2" s="890"/>
+      <c r="CV2" s="890" t="s">
         <v>260</v>
       </c>
-      <c r="CW2" s="853"/>
+      <c r="CW2" s="891"/>
     </row>
     <row r="3" spans="1:104" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="170"/>
@@ -60393,29 +60445,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="39">
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="CC1:CN1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AG1:AN1"/>
-    <mergeCell ref="AO1:AO2"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AT1:BV1"/>
-    <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
     <mergeCell ref="CP1:CW1"/>
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="CV2:CW2"/>
@@ -60432,6 +60461,29 @@
     <mergeCell ref="CT2:CU2"/>
     <mergeCell ref="CB1:CB2"/>
     <mergeCell ref="BX1:CA1"/>
+    <mergeCell ref="CC1:CN1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AG1:AN1"/>
+    <mergeCell ref="AO1:AO2"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AT1:BV1"/>
+    <mergeCell ref="BW1:BW2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -60474,105 +60526,110 @@
       <c r="K1" s="146"/>
       <c r="L1" s="147"/>
       <c r="M1" s="718"/>
-      <c r="N1" s="873"/>
-      <c r="O1" s="874"/>
-      <c r="P1" s="874"/>
-      <c r="Q1" s="874"/>
-      <c r="R1" s="875"/>
-      <c r="S1" s="868"/>
-      <c r="T1" s="868"/>
-      <c r="U1" s="868"/>
-      <c r="V1" s="868"/>
-      <c r="W1" s="868"/>
-      <c r="X1" s="876"/>
-      <c r="Y1" s="862"/>
-      <c r="Z1" s="832"/>
+      <c r="N1" s="862"/>
+      <c r="O1" s="863"/>
+      <c r="P1" s="863"/>
+      <c r="Q1" s="863"/>
+      <c r="R1" s="864"/>
+      <c r="S1" s="865"/>
+      <c r="T1" s="865"/>
+      <c r="U1" s="865"/>
+      <c r="V1" s="865"/>
+      <c r="W1" s="865"/>
+      <c r="X1" s="866"/>
+      <c r="Y1" s="867"/>
+      <c r="Z1" s="856"/>
       <c r="AA1" s="719"/>
       <c r="AB1" s="717"/>
-      <c r="AC1" s="864"/>
-      <c r="AD1" s="865"/>
-      <c r="AE1" s="865"/>
-      <c r="AF1" s="866"/>
-      <c r="AG1" s="867"/>
-      <c r="AH1" s="868"/>
-      <c r="AI1" s="868"/>
-      <c r="AJ1" s="868"/>
-      <c r="AK1" s="868"/>
-      <c r="AL1" s="868"/>
-      <c r="AM1" s="868"/>
-      <c r="AN1" s="868"/>
+      <c r="AC1" s="877"/>
+      <c r="AD1" s="878"/>
+      <c r="AE1" s="878"/>
+      <c r="AF1" s="879"/>
+      <c r="AG1" s="880"/>
+      <c r="AH1" s="865"/>
+      <c r="AI1" s="865"/>
+      <c r="AJ1" s="865"/>
+      <c r="AK1" s="865"/>
+      <c r="AL1" s="865"/>
+      <c r="AM1" s="865"/>
+      <c r="AN1" s="865"/>
       <c r="AO1" s="717"/>
-      <c r="AP1" s="862"/>
-      <c r="AQ1" s="832"/>
-      <c r="AR1" s="832"/>
-      <c r="AS1" s="833"/>
-      <c r="AT1" s="870"/>
-      <c r="AU1" s="871"/>
-      <c r="AV1" s="871"/>
-      <c r="AW1" s="871"/>
-      <c r="AX1" s="871"/>
-      <c r="AY1" s="871"/>
-      <c r="AZ1" s="871"/>
-      <c r="BA1" s="871"/>
-      <c r="BB1" s="871"/>
-      <c r="BC1" s="871"/>
-      <c r="BD1" s="871"/>
-      <c r="BE1" s="871"/>
-      <c r="BF1" s="871"/>
-      <c r="BG1" s="871"/>
-      <c r="BH1" s="871"/>
-      <c r="BI1" s="871"/>
-      <c r="BJ1" s="871"/>
-      <c r="BK1" s="871"/>
-      <c r="BL1" s="871"/>
-      <c r="BM1" s="871"/>
-      <c r="BN1" s="871"/>
-      <c r="BO1" s="871"/>
-      <c r="BP1" s="871"/>
-      <c r="BQ1" s="871"/>
-      <c r="BR1" s="871"/>
-      <c r="BS1" s="871"/>
-      <c r="BT1" s="871"/>
-      <c r="BU1" s="871"/>
-      <c r="BV1" s="871"/>
+      <c r="AP1" s="867"/>
+      <c r="AQ1" s="856"/>
+      <c r="AR1" s="856"/>
+      <c r="AS1" s="857"/>
+      <c r="AT1" s="884"/>
+      <c r="AU1" s="885"/>
+      <c r="AV1" s="885"/>
+      <c r="AW1" s="885"/>
+      <c r="AX1" s="885"/>
+      <c r="AY1" s="885"/>
+      <c r="AZ1" s="885"/>
+      <c r="BA1" s="885"/>
+      <c r="BB1" s="885"/>
+      <c r="BC1" s="885"/>
+      <c r="BD1" s="885"/>
+      <c r="BE1" s="885"/>
+      <c r="BF1" s="885"/>
+      <c r="BG1" s="885"/>
+      <c r="BH1" s="885"/>
+      <c r="BI1" s="885"/>
+      <c r="BJ1" s="885"/>
+      <c r="BK1" s="885"/>
+      <c r="BL1" s="885"/>
+      <c r="BM1" s="885"/>
+      <c r="BN1" s="885"/>
+      <c r="BO1" s="885"/>
+      <c r="BP1" s="885"/>
+      <c r="BQ1" s="885"/>
+      <c r="BR1" s="885"/>
+      <c r="BS1" s="885"/>
+      <c r="BT1" s="885"/>
+      <c r="BU1" s="885"/>
+      <c r="BV1" s="885"/>
       <c r="BW1" s="717"/>
-      <c r="BX1" s="862"/>
-      <c r="BY1" s="832"/>
-      <c r="BZ1" s="832"/>
-      <c r="CA1" s="833"/>
-      <c r="CB1" s="863"/>
-      <c r="CC1" s="863"/>
-      <c r="CD1" s="863"/>
-      <c r="CE1" s="863"/>
-      <c r="CF1" s="863"/>
-      <c r="CG1" s="863"/>
-      <c r="CH1" s="863"/>
-      <c r="CI1" s="863"/>
-      <c r="CJ1" s="863"/>
-      <c r="CK1" s="863"/>
-      <c r="CL1" s="863"/>
-      <c r="CM1" s="863"/>
+      <c r="BX1" s="867"/>
+      <c r="BY1" s="856"/>
+      <c r="BZ1" s="856"/>
+      <c r="CA1" s="857"/>
+      <c r="CB1" s="875"/>
+      <c r="CC1" s="875"/>
+      <c r="CD1" s="875"/>
+      <c r="CE1" s="875"/>
+      <c r="CF1" s="875"/>
+      <c r="CG1" s="875"/>
+      <c r="CH1" s="875"/>
+      <c r="CI1" s="875"/>
+      <c r="CJ1" s="875"/>
+      <c r="CK1" s="875"/>
+      <c r="CL1" s="875"/>
+      <c r="CM1" s="875"/>
       <c r="CN1" s="716"/>
-      <c r="CO1" s="849"/>
-      <c r="CP1" s="820"/>
-      <c r="CQ1" s="820"/>
-      <c r="CR1" s="820"/>
-      <c r="CS1" s="820"/>
-      <c r="CT1" s="820"/>
-      <c r="CU1" s="820"/>
-      <c r="CV1" s="821"/>
-      <c r="CW1" s="882"/>
-      <c r="CX1" s="883"/>
-      <c r="CY1" s="883"/>
-      <c r="CZ1" s="884"/>
-      <c r="DA1" s="883"/>
-      <c r="DB1" s="883"/>
-      <c r="DC1" s="884"/>
-      <c r="DD1" s="883"/>
-      <c r="DE1" s="883"/>
+      <c r="CO1" s="889"/>
+      <c r="CP1" s="826"/>
+      <c r="CQ1" s="826"/>
+      <c r="CR1" s="826"/>
+      <c r="CS1" s="826"/>
+      <c r="CT1" s="826"/>
+      <c r="CU1" s="826"/>
+      <c r="CV1" s="845"/>
+      <c r="CW1" s="894"/>
+      <c r="CX1" s="895"/>
+      <c r="CY1" s="895"/>
+      <c r="CZ1" s="896"/>
+      <c r="DA1" s="895"/>
+      <c r="DB1" s="895"/>
+      <c r="DC1" s="896"/>
+      <c r="DD1" s="895"/>
+      <c r="DE1" s="895"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="BX1:CA1"/>
+    <mergeCell ref="CB1:CM1"/>
     <mergeCell ref="CW1:CY1"/>
     <mergeCell ref="CZ1:DB1"/>
     <mergeCell ref="DC1:DE1"/>
@@ -60581,11 +60638,6 @@
     <mergeCell ref="AG1:AN1"/>
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:BV1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="BX1:CA1"/>
-    <mergeCell ref="CB1:CM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -60608,12 +60660,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="887" t="s">
+      <c r="A1" s="899" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="888"/>
-      <c r="C1" s="888"/>
-      <c r="D1" s="885" t="s">
+      <c r="B1" s="900"/>
+      <c r="C1" s="900"/>
+      <c r="D1" s="897" t="s">
         <v>263</v>
       </c>
     </row>
@@ -60627,7 +60679,7 @@
       <c r="C2" s="479" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="886"/>
+      <c r="D2" s="898"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="470"/>
@@ -60715,10 +60767,10 @@
       <c r="B2" s="205" t="s">
         <v>280</v>
       </c>
-      <c r="C2" s="896" t="s">
+      <c r="C2" s="901" t="s">
         <v>281</v>
       </c>
-      <c r="D2" s="896"/>
+      <c r="D2" s="901"/>
       <c r="E2" s="203"/>
       <c r="F2" s="203"/>
       <c r="G2" s="203"/>
@@ -60843,32 +60895,32 @@
     </row>
     <row r="7" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="202"/>
-      <c r="B7" s="897" t="s">
+      <c r="B7" s="902" t="s">
         <v>504</v>
       </c>
-      <c r="C7" s="897"/>
-      <c r="D7" s="897"/>
+      <c r="C7" s="902"/>
+      <c r="D7" s="902"/>
       <c r="E7" s="203"/>
       <c r="F7" s="203"/>
       <c r="G7" s="203"/>
       <c r="H7" s="203"/>
       <c r="I7" s="203"/>
-      <c r="J7" s="897" t="s">
+      <c r="J7" s="902" t="s">
         <v>503</v>
       </c>
-      <c r="K7" s="897"/>
-      <c r="L7" s="897"/>
+      <c r="K7" s="902"/>
+      <c r="L7" s="902"/>
       <c r="M7" s="203"/>
       <c r="N7" s="203"/>
       <c r="O7" s="203"/>
       <c r="P7" s="204" t="s">
         <v>285</v>
       </c>
-      <c r="Q7" s="897" t="s">
+      <c r="Q7" s="902" t="s">
         <v>504</v>
       </c>
-      <c r="R7" s="897"/>
-      <c r="S7" s="897"/>
+      <c r="R7" s="902"/>
+      <c r="S7" s="902"/>
       <c r="T7" s="203"/>
       <c r="U7" s="217" t="s">
         <v>286</v>
@@ -60902,41 +60954,41 @@
       <c r="B9" s="218" t="s">
         <v>506</v>
       </c>
-      <c r="C9" s="892" t="s">
+      <c r="C9" s="903" t="s">
         <v>287</v>
       </c>
-      <c r="D9" s="893"/>
-      <c r="E9" s="892" t="s">
+      <c r="D9" s="904"/>
+      <c r="E9" s="903" t="s">
         <v>288</v>
       </c>
-      <c r="F9" s="893"/>
+      <c r="F9" s="904"/>
       <c r="G9" s="203"/>
       <c r="H9" s="203"/>
       <c r="I9" s="203"/>
       <c r="J9" s="218" t="s">
         <v>506</v>
       </c>
-      <c r="K9" s="892" t="s">
+      <c r="K9" s="903" t="s">
         <v>287</v>
       </c>
-      <c r="L9" s="893"/>
-      <c r="M9" s="892" t="s">
+      <c r="L9" s="904"/>
+      <c r="M9" s="903" t="s">
         <v>288</v>
       </c>
-      <c r="N9" s="893"/>
+      <c r="N9" s="904"/>
       <c r="O9" s="203"/>
       <c r="P9" s="203"/>
       <c r="Q9" s="218" t="s">
         <v>506</v>
       </c>
-      <c r="R9" s="892" t="s">
+      <c r="R9" s="903" t="s">
         <v>287</v>
       </c>
-      <c r="S9" s="893"/>
-      <c r="T9" s="892" t="s">
+      <c r="S9" s="904"/>
+      <c r="T9" s="903" t="s">
         <v>288</v>
       </c>
-      <c r="U9" s="893"/>
+      <c r="U9" s="904"/>
     </row>
     <row r="10" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="202"/>
@@ -60998,10 +61050,10 @@
       </c>
       <c r="C11" s="223"/>
       <c r="D11" s="223"/>
-      <c r="E11" s="889" t="s">
+      <c r="E11" s="905" t="s">
         <v>292</v>
       </c>
-      <c r="F11" s="890"/>
+      <c r="F11" s="906"/>
       <c r="G11" s="224"/>
       <c r="H11" s="224"/>
       <c r="I11" s="224"/>
@@ -61010,10 +61062,10 @@
       </c>
       <c r="K11" s="203"/>
       <c r="L11" s="203"/>
-      <c r="M11" s="894" t="s">
+      <c r="M11" s="908" t="s">
         <v>292</v>
       </c>
-      <c r="N11" s="895"/>
+      <c r="N11" s="909"/>
       <c r="O11" s="224"/>
       <c r="P11" s="224"/>
       <c r="Q11" s="222" t="s">
@@ -61021,10 +61073,10 @@
       </c>
       <c r="R11" s="223"/>
       <c r="S11" s="223"/>
-      <c r="T11" s="889" t="s">
+      <c r="T11" s="905" t="s">
         <v>292</v>
       </c>
-      <c r="U11" s="890"/>
+      <c r="U11" s="906"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="202"/>
@@ -61259,10 +61311,10 @@
       </c>
       <c r="C20" s="304"/>
       <c r="D20" s="251"/>
-      <c r="E20" s="889" t="s">
+      <c r="E20" s="905" t="s">
         <v>299</v>
       </c>
-      <c r="F20" s="890"/>
+      <c r="F20" s="906"/>
       <c r="G20" s="232"/>
       <c r="H20" s="232"/>
       <c r="I20" s="203"/>
@@ -61271,10 +61323,10 @@
       </c>
       <c r="K20" s="304"/>
       <c r="L20" s="251"/>
-      <c r="M20" s="889" t="s">
+      <c r="M20" s="905" t="s">
         <v>299</v>
       </c>
-      <c r="N20" s="890"/>
+      <c r="N20" s="906"/>
       <c r="O20" s="242"/>
       <c r="P20" s="242"/>
       <c r="Q20" s="222" t="s">
@@ -61282,10 +61334,10 @@
       </c>
       <c r="R20" s="304"/>
       <c r="S20" s="251"/>
-      <c r="T20" s="889" t="s">
+      <c r="T20" s="905" t="s">
         <v>299</v>
       </c>
-      <c r="U20" s="890"/>
+      <c r="U20" s="906"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="202"/>
@@ -61549,10 +61601,10 @@
       </c>
       <c r="C30" s="304"/>
       <c r="D30" s="251"/>
-      <c r="E30" s="889" t="s">
+      <c r="E30" s="905" t="s">
         <v>299</v>
       </c>
-      <c r="F30" s="890"/>
+      <c r="F30" s="906"/>
       <c r="G30" s="232"/>
       <c r="H30" s="232"/>
       <c r="I30" s="203"/>
@@ -61561,10 +61613,10 @@
       </c>
       <c r="K30" s="304"/>
       <c r="L30" s="251"/>
-      <c r="M30" s="889" t="s">
+      <c r="M30" s="905" t="s">
         <v>299</v>
       </c>
-      <c r="N30" s="890"/>
+      <c r="N30" s="906"/>
       <c r="O30" s="242"/>
       <c r="P30" s="242"/>
       <c r="Q30" s="222" t="s">
@@ -61572,10 +61624,10 @@
       </c>
       <c r="R30" s="304"/>
       <c r="S30" s="251"/>
-      <c r="T30" s="889" t="s">
+      <c r="T30" s="905" t="s">
         <v>299</v>
       </c>
-      <c r="U30" s="890"/>
+      <c r="U30" s="906"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" s="264"/>
@@ -61898,11 +61950,11 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="202"/>
-      <c r="B42" s="891"/>
-      <c r="C42" s="891"/>
-      <c r="D42" s="891"/>
-      <c r="E42" s="891"/>
-      <c r="F42" s="891"/>
+      <c r="B42" s="907"/>
+      <c r="C42" s="907"/>
+      <c r="D42" s="907"/>
+      <c r="E42" s="907"/>
+      <c r="F42" s="907"/>
       <c r="G42" s="242"/>
       <c r="H42" s="203"/>
       <c r="I42" s="242"/>
@@ -62047,15 +62099,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="20">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="R9:S9"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="T30:U30"/>
@@ -62067,6 +62110,15 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="T20:U20"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="R9:S9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>